<commit_message>
error al inicializar popo_citizens
home en vez de Home
</commit_message>
<xml_diff>
--- a/data/Otxarkoaga/population/pop_building.xlsx
+++ b/data/Otxarkoaga/population/pop_building.xlsx
@@ -3065,16 +3065,16 @@
         </is>
       </c>
       <c r="G60" t="n">
-        <v>460.1631726545987</v>
+        <v>425.6199974785681</v>
       </c>
       <c r="H60" t="n">
-        <v>1130.172836787981</v>
+        <v>1109.81909692339</v>
       </c>
       <c r="I60" t="n">
-        <v>553.5659160591301</v>
+        <v>488.7549500135832</v>
       </c>
       <c r="J60" t="n">
-        <v>1130.172836787981</v>
+        <v>1109.81909692339</v>
       </c>
     </row>
     <row r="61">
@@ -3105,13 +3105,13 @@
         </is>
       </c>
       <c r="G61" t="n">
-        <v>420</v>
+        <v>484.3341223874794</v>
       </c>
       <c r="H61" t="n">
         <v>1060</v>
       </c>
       <c r="I61" t="n">
-        <v>450.7945633853931</v>
+        <v>530.2982239905306</v>
       </c>
       <c r="J61" t="n">
         <v>1060</v>
@@ -3145,16 +3145,16 @@
         </is>
       </c>
       <c r="G62" t="n">
-        <v>420</v>
+        <v>441.4392373202759</v>
       </c>
       <c r="H62" t="n">
-        <v>1121.897848669869</v>
+        <v>1060</v>
       </c>
       <c r="I62" t="n">
-        <v>516.2806167237669</v>
+        <v>541.7930332231717</v>
       </c>
       <c r="J62" t="n">
-        <v>1121.897848669869</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="63">
@@ -3185,16 +3185,16 @@
         </is>
       </c>
       <c r="G63" t="n">
-        <v>484.3867054126716</v>
+        <v>452.1935299360994</v>
       </c>
       <c r="H63" t="n">
-        <v>1064.09685869723</v>
+        <v>1061.545585087516</v>
       </c>
       <c r="I63" t="n">
-        <v>526.5446771829562</v>
+        <v>502.6308710596613</v>
       </c>
       <c r="J63" t="n">
-        <v>1064.09685869723</v>
+        <v>1061.545585087516</v>
       </c>
     </row>
     <row r="64">
@@ -3225,16 +3225,16 @@
         </is>
       </c>
       <c r="G64" t="n">
-        <v>428.4784583191139</v>
+        <v>420</v>
       </c>
       <c r="H64" t="n">
-        <v>1108.87769036292</v>
+        <v>1131.922984461146</v>
       </c>
       <c r="I64" t="n">
-        <v>548.1781458520518</v>
+        <v>456.3772072549711</v>
       </c>
       <c r="J64" t="n">
-        <v>1108.87769036292</v>
+        <v>1131.922984461146</v>
       </c>
     </row>
     <row r="65">
@@ -3265,16 +3265,16 @@
         </is>
       </c>
       <c r="G65" t="n">
-        <v>463.3512207278483</v>
+        <v>486.7059351889586</v>
       </c>
       <c r="H65" t="n">
-        <v>1105.127438667506</v>
+        <v>1060</v>
       </c>
       <c r="I65" t="n">
-        <v>504.8649911519651</v>
+        <v>562.0362784977859</v>
       </c>
       <c r="J65" t="n">
-        <v>1105.127438667506</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="66">
@@ -3305,16 +3305,16 @@
         </is>
       </c>
       <c r="G66" t="n">
-        <v>420</v>
+        <v>448.7945382386145</v>
       </c>
       <c r="H66" t="n">
-        <v>1118.110039096906</v>
+        <v>1093.034705620703</v>
       </c>
       <c r="I66" t="n">
-        <v>446.0673995193226</v>
+        <v>458.8722132280118</v>
       </c>
       <c r="J66" t="n">
-        <v>1118.110039096906</v>
+        <v>1093.034705620703</v>
       </c>
     </row>
     <row r="67">
@@ -3345,16 +3345,16 @@
         </is>
       </c>
       <c r="G67" t="n">
-        <v>468.6721060769898</v>
+        <v>474.5854885093802</v>
       </c>
       <c r="H67" t="n">
-        <v>1083.130740424688</v>
+        <v>1102.418640316122</v>
       </c>
       <c r="I67" t="n">
-        <v>544.1555920903513</v>
+        <v>493.6266222359977</v>
       </c>
       <c r="J67" t="n">
-        <v>1083.130740424688</v>
+        <v>1102.418640316122</v>
       </c>
     </row>
     <row r="68">
@@ -3385,16 +3385,16 @@
         </is>
       </c>
       <c r="G68" t="n">
-        <v>478.8468806373893</v>
+        <v>440.5405962937811</v>
       </c>
       <c r="H68" t="n">
-        <v>1095.777357007235</v>
+        <v>1086.113437186111</v>
       </c>
       <c r="I68" t="n">
-        <v>566.6067836353023</v>
+        <v>541.3548569860993</v>
       </c>
       <c r="J68" t="n">
-        <v>1095.777357007235</v>
+        <v>1086.113437186111</v>
       </c>
     </row>
     <row r="69">
@@ -3425,16 +3425,16 @@
         </is>
       </c>
       <c r="G69" t="n">
-        <v>450.5089811816255</v>
+        <v>461.1170142547982</v>
       </c>
       <c r="H69" t="n">
-        <v>1222.49760408647</v>
+        <v>1281.308066815435</v>
       </c>
       <c r="I69" t="n">
-        <v>516.1266217897194</v>
+        <v>468.6150451318845</v>
       </c>
       <c r="J69" t="n">
-        <v>1222.49760408647</v>
+        <v>1281.308066815435</v>
       </c>
     </row>
     <row r="70">
@@ -3465,16 +3465,16 @@
         </is>
       </c>
       <c r="G70" t="n">
-        <v>455.5643176519884</v>
+        <v>525.8686705755246</v>
       </c>
       <c r="H70" t="n">
-        <v>1308.533811975337</v>
+        <v>1176.413156887814</v>
       </c>
       <c r="I70" t="n">
-        <v>511.1460192358177</v>
+        <v>570.0616721818711</v>
       </c>
       <c r="J70" t="n">
-        <v>1308.533811975337</v>
+        <v>1176.413156887814</v>
       </c>
     </row>
     <row r="71">
@@ -3505,16 +3505,16 @@
         </is>
       </c>
       <c r="G71" t="n">
-        <v>459.5955058060196</v>
+        <v>517.8981423842758</v>
       </c>
       <c r="H71" t="n">
-        <v>1320</v>
+        <v>1282.994780038358</v>
       </c>
       <c r="I71" t="n">
-        <v>530.4952576337387</v>
+        <v>581.2803879100582</v>
       </c>
       <c r="J71" t="n">
-        <v>1320</v>
+        <v>1282.994780038358</v>
       </c>
     </row>
     <row r="72">
@@ -3545,16 +3545,16 @@
         </is>
       </c>
       <c r="G72" t="n">
-        <v>531.4432621814303</v>
+        <v>492.5022711832751</v>
       </c>
       <c r="H72" t="n">
-        <v>1309.901715219128</v>
+        <v>1320</v>
       </c>
       <c r="I72" t="n">
-        <v>584.997526142279</v>
+        <v>593.4539102557748</v>
       </c>
       <c r="J72" t="n">
-        <v>1309.901715219128</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="73">
@@ -3585,16 +3585,16 @@
         </is>
       </c>
       <c r="G73" t="n">
-        <v>493.7115956911861</v>
+        <v>500.4678341046388</v>
       </c>
       <c r="H73" t="n">
-        <v>1233.268977593717</v>
+        <v>1224.181282280326</v>
       </c>
       <c r="I73" t="n">
-        <v>530.0018797725759</v>
+        <v>553.5753285438309</v>
       </c>
       <c r="J73" t="n">
-        <v>1233.268977593717</v>
+        <v>1224.181282280326</v>
       </c>
     </row>
     <row r="74">
@@ -3625,16 +3625,16 @@
         </is>
       </c>
       <c r="G74" t="n">
-        <v>527.7090561612222</v>
+        <v>434.2955056022997</v>
       </c>
       <c r="H74" t="n">
-        <v>1262.13559795787</v>
+        <v>1269.503486543706</v>
       </c>
       <c r="I74" t="n">
-        <v>612.8343542800754</v>
+        <v>545.7078446187787</v>
       </c>
       <c r="J74" t="n">
-        <v>1262.13559795787</v>
+        <v>1269.503486543706</v>
       </c>
     </row>
     <row r="75">
@@ -3665,16 +3665,16 @@
         </is>
       </c>
       <c r="G75" t="n">
-        <v>486.7369722959769</v>
+        <v>474.0308815501552</v>
       </c>
       <c r="H75" t="n">
-        <v>1282.159387224075</v>
+        <v>1230.552887388359</v>
       </c>
       <c r="I75" t="n">
-        <v>541.2008217071754</v>
+        <v>527.8663272849549</v>
       </c>
       <c r="J75" t="n">
-        <v>1282.159387224075</v>
+        <v>1230.552887388359</v>
       </c>
     </row>
     <row r="76">
@@ -3708,13 +3708,13 @@
         <v>540</v>
       </c>
       <c r="H76" t="n">
-        <v>1212.960606368029</v>
+        <v>1286.785940718925</v>
       </c>
       <c r="I76" t="n">
-        <v>588.480510965402</v>
+        <v>660</v>
       </c>
       <c r="J76" t="n">
-        <v>1212.960606368029</v>
+        <v>1286.785940718925</v>
       </c>
     </row>
     <row r="77">
@@ -3745,16 +3745,16 @@
         </is>
       </c>
       <c r="G77" t="n">
-        <v>420</v>
+        <v>428.1153792110128</v>
       </c>
       <c r="H77" t="n">
-        <v>1193.11481292863</v>
+        <v>1320</v>
       </c>
       <c r="I77" t="n">
-        <v>459.7340517089737</v>
+        <v>481.3229063003999</v>
       </c>
       <c r="J77" t="n">
-        <v>1193.11481292863</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="78">
@@ -3785,16 +3785,16 @@
         </is>
       </c>
       <c r="G78" t="n">
-        <v>466.1142361697176</v>
+        <v>434.9680898387795</v>
       </c>
       <c r="H78" t="n">
-        <v>1241.627959018567</v>
+        <v>1272.531443361663</v>
       </c>
       <c r="I78" t="n">
-        <v>530.5431794033825</v>
+        <v>513.5164476963356</v>
       </c>
       <c r="J78" t="n">
-        <v>1241.627959018567</v>
+        <v>1272.531443361663</v>
       </c>
     </row>
     <row r="79">
@@ -3825,16 +3825,16 @@
         </is>
       </c>
       <c r="G79" t="n">
-        <v>505.285838682494</v>
+        <v>429.8896967555555</v>
       </c>
       <c r="H79" t="n">
-        <v>1203.657784863796</v>
+        <v>1320</v>
       </c>
       <c r="I79" t="n">
-        <v>527.6270793683832</v>
+        <v>521.6389061639875</v>
       </c>
       <c r="J79" t="n">
-        <v>1203.657784863796</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="80">
@@ -3865,16 +3865,16 @@
         </is>
       </c>
       <c r="G80" t="n">
-        <v>484.4722716382864</v>
+        <v>494.656747729738</v>
       </c>
       <c r="H80" t="n">
-        <v>1235.497506726384</v>
+        <v>1320</v>
       </c>
       <c r="I80" t="n">
-        <v>513.0373424006219</v>
+        <v>562.2589866162052</v>
       </c>
       <c r="J80" t="n">
-        <v>1235.497506726384</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="81">
@@ -3905,16 +3905,16 @@
         </is>
       </c>
       <c r="G81" t="n">
-        <v>466.5506249602017</v>
+        <v>466.8235572255791</v>
       </c>
       <c r="H81" t="n">
-        <v>1226.456107553024</v>
+        <v>1193.154541366167</v>
       </c>
       <c r="I81" t="n">
-        <v>574.0465360015817</v>
+        <v>468.1118237558955</v>
       </c>
       <c r="J81" t="n">
-        <v>1226.456107553024</v>
+        <v>1193.154541366167</v>
       </c>
     </row>
     <row r="82">
@@ -3945,16 +3945,16 @@
         </is>
       </c>
       <c r="G82" t="n">
-        <v>501.5656195110118</v>
+        <v>488.7652522169874</v>
       </c>
       <c r="H82" t="n">
-        <v>1320</v>
+        <v>1133.320286013789</v>
       </c>
       <c r="I82" t="n">
-        <v>501.5656195110118</v>
+        <v>488.7652522169874</v>
       </c>
       <c r="J82" t="n">
-        <v>1320</v>
+        <v>1133.320286013789</v>
       </c>
     </row>
     <row r="83">
@@ -3985,16 +3985,16 @@
         </is>
       </c>
       <c r="G83" t="n">
-        <v>494.1841180069736</v>
+        <v>520.5417811676833</v>
       </c>
       <c r="H83" t="n">
-        <v>1320</v>
+        <v>1236.225079544521</v>
       </c>
       <c r="I83" t="n">
-        <v>494.1841180069736</v>
+        <v>520.5417811676833</v>
       </c>
       <c r="J83" t="n">
-        <v>1320</v>
+        <v>1236.225079544521</v>
       </c>
     </row>
     <row r="84">
@@ -4025,16 +4025,16 @@
         </is>
       </c>
       <c r="G84" t="n">
-        <v>524.1958910919742</v>
+        <v>498.759920070242</v>
       </c>
       <c r="H84" t="n">
-        <v>1266.354205334919</v>
+        <v>1314.659401594806</v>
       </c>
       <c r="I84" t="n">
-        <v>524.1958910919742</v>
+        <v>498.759920070242</v>
       </c>
       <c r="J84" t="n">
-        <v>1266.354205334919</v>
+        <v>1314.659401594806</v>
       </c>
     </row>
     <row r="85">
@@ -4065,16 +4065,16 @@
         </is>
       </c>
       <c r="G85" t="n">
-        <v>512.5479985528992</v>
+        <v>492.8863058849175</v>
       </c>
       <c r="H85" t="n">
-        <v>1320</v>
+        <v>1250.535866987504</v>
       </c>
       <c r="I85" t="n">
-        <v>512.5479985528992</v>
+        <v>492.8863058849175</v>
       </c>
       <c r="J85" t="n">
-        <v>1320</v>
+        <v>1250.535866987504</v>
       </c>
     </row>
     <row r="86">
@@ -4105,16 +4105,16 @@
         </is>
       </c>
       <c r="G86" t="n">
-        <v>467.2098942013323</v>
+        <v>473.9417294651641</v>
       </c>
       <c r="H86" t="n">
-        <v>1132.651031462346</v>
+        <v>1235.240927559497</v>
       </c>
       <c r="I86" t="n">
-        <v>467.2098942013323</v>
+        <v>473.9417294651641</v>
       </c>
       <c r="J86" t="n">
-        <v>1132.651031462346</v>
+        <v>1235.240927559497</v>
       </c>
     </row>
     <row r="87">
@@ -4145,16 +4145,16 @@
         </is>
       </c>
       <c r="G87" t="n">
-        <v>496.1570031384559</v>
+        <v>510.894816117106</v>
       </c>
       <c r="H87" t="n">
-        <v>1277.145426917592</v>
+        <v>1275.51436535502</v>
       </c>
       <c r="I87" t="n">
-        <v>496.1570031384559</v>
+        <v>510.894816117106</v>
       </c>
       <c r="J87" t="n">
-        <v>1277.145426917592</v>
+        <v>1275.51436535502</v>
       </c>
     </row>
     <row r="88">
@@ -4185,16 +4185,16 @@
         </is>
       </c>
       <c r="G88" t="n">
-        <v>524.9969137315647</v>
+        <v>530.7321297828119</v>
       </c>
       <c r="H88" t="n">
-        <v>1320</v>
+        <v>1224.719232873604</v>
       </c>
       <c r="I88" t="n">
-        <v>524.9969137315647</v>
+        <v>530.7321297828119</v>
       </c>
       <c r="J88" t="n">
-        <v>1320</v>
+        <v>1224.719232873604</v>
       </c>
     </row>
     <row r="89">
@@ -4225,16 +4225,16 @@
         </is>
       </c>
       <c r="G89" t="n">
-        <v>459.902067755896</v>
+        <v>540</v>
       </c>
       <c r="H89" t="n">
-        <v>1246.253505836918</v>
+        <v>1160.311147533977</v>
       </c>
       <c r="I89" t="n">
-        <v>459.902067755896</v>
+        <v>540</v>
       </c>
       <c r="J89" t="n">
-        <v>1246.253505836918</v>
+        <v>1160.311147533977</v>
       </c>
     </row>
     <row r="90">
@@ -4265,16 +4265,16 @@
         </is>
       </c>
       <c r="G90" t="n">
-        <v>540</v>
+        <v>478.7276862717181</v>
       </c>
       <c r="H90" t="n">
-        <v>1320</v>
+        <v>1250.262218651491</v>
       </c>
       <c r="I90" t="n">
-        <v>540</v>
+        <v>478.7276862717181</v>
       </c>
       <c r="J90" t="n">
-        <v>1320</v>
+        <v>1250.262218651491</v>
       </c>
     </row>
     <row r="91">
@@ -4305,16 +4305,16 @@
         </is>
       </c>
       <c r="G91" t="n">
-        <v>497.3129073631059</v>
+        <v>528.5983969224268</v>
       </c>
       <c r="H91" t="n">
-        <v>1287.253944932987</v>
+        <v>1184.392696575258</v>
       </c>
       <c r="I91" t="n">
-        <v>497.3129073631059</v>
+        <v>528.5983969224268</v>
       </c>
       <c r="J91" t="n">
-        <v>1287.253944932987</v>
+        <v>1184.392696575258</v>
       </c>
     </row>
     <row r="92">
@@ -4345,16 +4345,16 @@
         </is>
       </c>
       <c r="G92" t="n">
-        <v>489.6232115888536</v>
+        <v>472.692481152121</v>
       </c>
       <c r="H92" t="n">
-        <v>1135.444158601067</v>
+        <v>1163.251296666992</v>
       </c>
       <c r="I92" t="n">
-        <v>489.6232115888536</v>
+        <v>472.692481152121</v>
       </c>
       <c r="J92" t="n">
-        <v>1135.444158601067</v>
+        <v>1163.251296666992</v>
       </c>
     </row>
     <row r="93">
@@ -4385,16 +4385,16 @@
         </is>
       </c>
       <c r="G93" t="n">
-        <v>484.6098165426479</v>
+        <v>530.0338837234964</v>
       </c>
       <c r="H93" t="n">
-        <v>1262.781125042167</v>
+        <v>1157.848153305914</v>
       </c>
       <c r="I93" t="n">
-        <v>484.6098165426479</v>
+        <v>530.0338837234964</v>
       </c>
       <c r="J93" t="n">
-        <v>1262.781125042167</v>
+        <v>1157.848153305914</v>
       </c>
     </row>
     <row r="94">
@@ -4425,16 +4425,16 @@
         </is>
       </c>
       <c r="G94" t="n">
-        <v>540</v>
+        <v>477.0826789483378</v>
       </c>
       <c r="H94" t="n">
-        <v>1302.861757988107</v>
+        <v>1301.259364409706</v>
       </c>
       <c r="I94" t="n">
-        <v>540</v>
+        <v>477.0826789483378</v>
       </c>
       <c r="J94" t="n">
-        <v>1302.861757988107</v>
+        <v>1301.259364409706</v>
       </c>
     </row>
     <row r="95">
@@ -4465,16 +4465,16 @@
         </is>
       </c>
       <c r="G95" t="n">
-        <v>490.7688537941043</v>
+        <v>505.2819891498899</v>
       </c>
       <c r="H95" t="n">
-        <v>1320</v>
+        <v>1247.041054379891</v>
       </c>
       <c r="I95" t="n">
-        <v>490.7688537941043</v>
+        <v>505.2819891498899</v>
       </c>
       <c r="J95" t="n">
-        <v>1320</v>
+        <v>1247.041054379891</v>
       </c>
     </row>
     <row r="96">
@@ -4508,13 +4508,13 @@
         <v>540</v>
       </c>
       <c r="H96" t="n">
-        <v>1320</v>
+        <v>1183.091075618762</v>
       </c>
       <c r="I96" t="n">
         <v>540</v>
       </c>
       <c r="J96" t="n">
-        <v>1320</v>
+        <v>1183.091075618762</v>
       </c>
     </row>
     <row r="97">
@@ -4545,16 +4545,16 @@
         </is>
       </c>
       <c r="G97" t="n">
-        <v>468.2025301508383</v>
+        <v>488.5099535507683</v>
       </c>
       <c r="H97" t="n">
-        <v>1320</v>
+        <v>1207.952119063593</v>
       </c>
       <c r="I97" t="n">
-        <v>468.2025301508383</v>
+        <v>488.5099535507683</v>
       </c>
       <c r="J97" t="n">
-        <v>1320</v>
+        <v>1207.952119063593</v>
       </c>
     </row>
     <row r="98">
@@ -4585,16 +4585,16 @@
         </is>
       </c>
       <c r="G98" t="n">
-        <v>525.9547917987898</v>
+        <v>506.9808142475516</v>
       </c>
       <c r="H98" t="n">
-        <v>1277.758462736059</v>
+        <v>1181.80796508218</v>
       </c>
       <c r="I98" t="n">
-        <v>525.9547917987898</v>
+        <v>506.9808142475516</v>
       </c>
       <c r="J98" t="n">
-        <v>1277.758462736059</v>
+        <v>1181.80796508218</v>
       </c>
     </row>
     <row r="99">
@@ -4625,16 +4625,16 @@
         </is>
       </c>
       <c r="G99" t="n">
-        <v>502.549501003777</v>
+        <v>540</v>
       </c>
       <c r="H99" t="n">
-        <v>1320</v>
+        <v>1187.36974110631</v>
       </c>
       <c r="I99" t="n">
-        <v>502.549501003777</v>
+        <v>540</v>
       </c>
       <c r="J99" t="n">
-        <v>1320</v>
+        <v>1187.36974110631</v>
       </c>
     </row>
     <row r="100">
@@ -4665,16 +4665,16 @@
         </is>
       </c>
       <c r="G100" t="n">
-        <v>506.9887379531892</v>
+        <v>515.5823409859667</v>
       </c>
       <c r="H100" t="n">
-        <v>1237.933285783602</v>
+        <v>1236.269823732114</v>
       </c>
       <c r="I100" t="n">
-        <v>506.9887379531892</v>
+        <v>515.5823409859667</v>
       </c>
       <c r="J100" t="n">
-        <v>1237.933285783602</v>
+        <v>1236.269823732114</v>
       </c>
     </row>
     <row r="101">
@@ -4705,16 +4705,16 @@
         </is>
       </c>
       <c r="G101" t="n">
-        <v>506.675600943113</v>
+        <v>501.8733502154853</v>
       </c>
       <c r="H101" t="n">
-        <v>1227.064846148421</v>
+        <v>1166.983240083073</v>
       </c>
       <c r="I101" t="n">
-        <v>506.675600943113</v>
+        <v>501.8733502154853</v>
       </c>
       <c r="J101" t="n">
-        <v>1227.064846148421</v>
+        <v>1166.983240083073</v>
       </c>
     </row>
     <row r="102">
@@ -4745,13 +4745,13 @@
         </is>
       </c>
       <c r="G102" t="n">
-        <v>524.59821058879</v>
+        <v>540</v>
       </c>
       <c r="H102" t="n">
         <v>1320</v>
       </c>
       <c r="I102" t="n">
-        <v>524.59821058879</v>
+        <v>540</v>
       </c>
       <c r="J102" t="n">
         <v>1320</v>
@@ -4785,16 +4785,16 @@
         </is>
       </c>
       <c r="G103" t="n">
-        <v>476.1935006709363</v>
+        <v>431.345332279926</v>
       </c>
       <c r="H103" t="n">
-        <v>1186.273685485914</v>
+        <v>1191.072948020083</v>
       </c>
       <c r="I103" t="n">
-        <v>476.1935006709363</v>
+        <v>431.345332279926</v>
       </c>
       <c r="J103" t="n">
-        <v>1186.273685485914</v>
+        <v>1191.072948020083</v>
       </c>
     </row>
     <row r="104">
@@ -4825,16 +4825,16 @@
         </is>
       </c>
       <c r="G104" t="n">
-        <v>528.1381810013676</v>
+        <v>507.1797743938082</v>
       </c>
       <c r="H104" t="n">
-        <v>1289.409500028883</v>
+        <v>1320</v>
       </c>
       <c r="I104" t="n">
-        <v>528.1381810013676</v>
+        <v>507.1797743938082</v>
       </c>
       <c r="J104" t="n">
-        <v>1289.409500028883</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="105">
@@ -4865,16 +4865,16 @@
         </is>
       </c>
       <c r="G105" t="n">
-        <v>462.512753593788</v>
+        <v>503.2908368097868</v>
       </c>
       <c r="H105" t="n">
-        <v>1279.067237465841</v>
+        <v>1320</v>
       </c>
       <c r="I105" t="n">
-        <v>462.512753593788</v>
+        <v>503.2908368097868</v>
       </c>
       <c r="J105" t="n">
-        <v>1279.067237465841</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="106">
@@ -4905,16 +4905,16 @@
         </is>
       </c>
       <c r="G106" t="n">
-        <v>526.3250918327703</v>
+        <v>492.7975468812764</v>
       </c>
       <c r="H106" t="n">
-        <v>1130.820835304121</v>
+        <v>1127.563397227397</v>
       </c>
       <c r="I106" t="n">
-        <v>526.3250918327703</v>
+        <v>492.7975468812764</v>
       </c>
       <c r="J106" t="n">
-        <v>1130.820835304121</v>
+        <v>1127.563397227397</v>
       </c>
     </row>
     <row r="107">
@@ -4945,16 +4945,16 @@
         </is>
       </c>
       <c r="G107" t="n">
-        <v>503.0402470492605</v>
+        <v>490.9291110666542</v>
       </c>
       <c r="H107" t="n">
-        <v>1242.341212991534</v>
+        <v>1023.348143811229</v>
       </c>
       <c r="I107" t="n">
-        <v>503.0402470492605</v>
+        <v>490.9291110666542</v>
       </c>
       <c r="J107" t="n">
-        <v>1242.341212991534</v>
+        <v>1023.348143811229</v>
       </c>
     </row>
     <row r="108">
@@ -4985,16 +4985,16 @@
         </is>
       </c>
       <c r="G108" t="n">
-        <v>478.2657360415095</v>
+        <v>477.1109014062662</v>
       </c>
       <c r="H108" t="n">
-        <v>1190.419259689994</v>
+        <v>1107.161280044805</v>
       </c>
       <c r="I108" t="n">
-        <v>478.2657360415095</v>
+        <v>477.1109014062662</v>
       </c>
       <c r="J108" t="n">
-        <v>1190.419259689994</v>
+        <v>1107.161280044805</v>
       </c>
     </row>
     <row r="109">
@@ -5025,16 +5025,16 @@
         </is>
       </c>
       <c r="G109" t="n">
-        <v>467.3256584996979</v>
+        <v>486.2784549696033</v>
       </c>
       <c r="H109" t="n">
-        <v>1301.771693929272</v>
+        <v>1207.084294160133</v>
       </c>
       <c r="I109" t="n">
-        <v>467.3256584996979</v>
+        <v>486.2784549696033</v>
       </c>
       <c r="J109" t="n">
-        <v>1301.771693929272</v>
+        <v>1207.084294160133</v>
       </c>
     </row>
     <row r="110">
@@ -5065,16 +5065,16 @@
         </is>
       </c>
       <c r="G110" t="n">
-        <v>518.8182463025443</v>
+        <v>487.0944389733001</v>
       </c>
       <c r="H110" t="n">
-        <v>1272.686740387732</v>
+        <v>1320</v>
       </c>
       <c r="I110" t="n">
-        <v>518.8182463025443</v>
+        <v>487.0944389733001</v>
       </c>
       <c r="J110" t="n">
-        <v>1272.686740387732</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="111">
@@ -5105,16 +5105,16 @@
         </is>
       </c>
       <c r="G111" t="n">
-        <v>521.6926643036666</v>
+        <v>472.5542081912803</v>
       </c>
       <c r="H111" t="n">
-        <v>1320</v>
+        <v>1273.518638255934</v>
       </c>
       <c r="I111" t="n">
-        <v>521.6926643036666</v>
+        <v>472.5542081912803</v>
       </c>
       <c r="J111" t="n">
-        <v>1320</v>
+        <v>1273.518638255934</v>
       </c>
     </row>
     <row r="112">
@@ -5145,16 +5145,16 @@
         </is>
       </c>
       <c r="G112" t="n">
-        <v>495.3225425551572</v>
+        <v>497.6905213055467</v>
       </c>
       <c r="H112" t="n">
-        <v>1320</v>
+        <v>1020</v>
       </c>
       <c r="I112" t="n">
-        <v>495.3225425551572</v>
+        <v>497.6905213055467</v>
       </c>
       <c r="J112" t="n">
-        <v>1320</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="113">
@@ -5188,13 +5188,13 @@
         <v>540</v>
       </c>
       <c r="H113" t="n">
-        <v>1085.716569264383</v>
+        <v>1320</v>
       </c>
       <c r="I113" t="n">
         <v>540</v>
       </c>
       <c r="J113" t="n">
-        <v>1085.716569264383</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="114">
@@ -5225,16 +5225,16 @@
         </is>
       </c>
       <c r="G114" t="n">
-        <v>472.4283102346498</v>
+        <v>523.1647634235019</v>
       </c>
       <c r="H114" t="n">
-        <v>1020</v>
+        <v>1422.897613135276</v>
       </c>
       <c r="I114" t="n">
-        <v>489.0443234175984</v>
+        <v>577.4887414565898</v>
       </c>
       <c r="J114" t="n">
-        <v>1020</v>
+        <v>1422.897613135276</v>
       </c>
     </row>
     <row r="115">
@@ -5265,16 +5265,16 @@
         </is>
       </c>
       <c r="G115" t="n">
-        <v>498.2169758487134</v>
+        <v>567.2571247657582</v>
       </c>
       <c r="H115" t="n">
-        <v>1440</v>
+        <v>1329.92820662964</v>
       </c>
       <c r="I115" t="n">
-        <v>598.9686300577511</v>
+        <v>677.8239854363669</v>
       </c>
       <c r="J115" t="n">
-        <v>1440</v>
+        <v>1329.92820662964</v>
       </c>
     </row>
     <row r="116">
@@ -5305,16 +5305,16 @@
         </is>
       </c>
       <c r="G116" t="n">
-        <v>464.418472207141</v>
+        <v>503.3125695587083</v>
       </c>
       <c r="H116" t="n">
-        <v>1439.8255524395</v>
+        <v>1044.192413349959</v>
       </c>
       <c r="I116" t="n">
-        <v>526.222274614858</v>
+        <v>561.3335937814069</v>
       </c>
       <c r="J116" t="n">
-        <v>1439.8255524395</v>
+        <v>1044.192413349959</v>
       </c>
     </row>
     <row r="117">
@@ -5345,16 +5345,16 @@
         </is>
       </c>
       <c r="G117" t="n">
-        <v>538.5544869658339</v>
+        <v>473.373561028697</v>
       </c>
       <c r="H117" t="n">
-        <v>1346.985673863689</v>
+        <v>1205.592605007651</v>
       </c>
       <c r="I117" t="n">
-        <v>538.5544869658339</v>
+        <v>566.9802907709251</v>
       </c>
       <c r="J117" t="n">
-        <v>1346.985673863689</v>
+        <v>1205.592605007651</v>
       </c>
     </row>
     <row r="118">
@@ -5391,7 +5391,7 @@
         <v>1020</v>
       </c>
       <c r="I118" t="n">
-        <v>441.4740850401467</v>
+        <v>480.5407492695625</v>
       </c>
       <c r="J118" t="n">
         <v>1020</v>
@@ -5428,13 +5428,13 @@
         <v>420</v>
       </c>
       <c r="H119" t="n">
-        <v>1166.465793658684</v>
+        <v>1371.703189544591</v>
       </c>
       <c r="I119" t="n">
-        <v>490.7120008016584</v>
+        <v>458.9940229612305</v>
       </c>
       <c r="J119" t="n">
-        <v>1166.465793658684</v>
+        <v>1371.703189544591</v>
       </c>
     </row>
     <row r="120">
@@ -5465,16 +5465,16 @@
         </is>
       </c>
       <c r="G120" t="n">
-        <v>501.7977696066882</v>
+        <v>421.4133206450233</v>
       </c>
       <c r="H120" t="n">
-        <v>1272.654029773502</v>
+        <v>1185.025511322994</v>
       </c>
       <c r="I120" t="n">
-        <v>561.859639497169</v>
+        <v>458.4326865885344</v>
       </c>
       <c r="J120" t="n">
-        <v>1272.654029773502</v>
+        <v>1185.025511322994</v>
       </c>
     </row>
     <row r="121">
@@ -5505,16 +5505,16 @@
         </is>
       </c>
       <c r="G121" t="n">
-        <v>466.9179104515876</v>
+        <v>463.6178296418903</v>
       </c>
       <c r="H121" t="n">
-        <v>1114.221968753446</v>
+        <v>1158.29083141603</v>
       </c>
       <c r="I121" t="n">
-        <v>484.8478461821626</v>
+        <v>517.5750056937503</v>
       </c>
       <c r="J121" t="n">
-        <v>1114.221968753446</v>
+        <v>1158.29083141603</v>
       </c>
     </row>
     <row r="122">
@@ -5545,13 +5545,13 @@
         </is>
       </c>
       <c r="G122" t="n">
-        <v>420</v>
+        <v>519.3236960590234</v>
       </c>
       <c r="H122" t="n">
         <v>1020</v>
       </c>
       <c r="I122" t="n">
-        <v>445.8875979796981</v>
+        <v>542.455227175305</v>
       </c>
       <c r="J122" t="n">
         <v>1020</v>
@@ -5585,16 +5585,16 @@
         </is>
       </c>
       <c r="G123" t="n">
-        <v>572.0543830922421</v>
+        <v>420</v>
       </c>
       <c r="H123" t="n">
-        <v>1020</v>
+        <v>1168.114825446693</v>
       </c>
       <c r="I123" t="n">
-        <v>612.3155068865738</v>
+        <v>527.8236435924736</v>
       </c>
       <c r="J123" t="n">
-        <v>1020</v>
+        <v>1168.114825446693</v>
       </c>
     </row>
     <row r="124">
@@ -5625,16 +5625,16 @@
         </is>
       </c>
       <c r="G124" t="n">
-        <v>485.9039518739248</v>
+        <v>475.9344095921315</v>
       </c>
       <c r="H124" t="n">
-        <v>1411.891341650135</v>
+        <v>1292.943641144439</v>
       </c>
       <c r="I124" t="n">
-        <v>506.5783590933253</v>
+        <v>504.1406296545287</v>
       </c>
       <c r="J124" t="n">
-        <v>1411.891341650135</v>
+        <v>1292.943641144439</v>
       </c>
     </row>
     <row r="125">
@@ -5665,16 +5665,16 @@
         </is>
       </c>
       <c r="G125" t="n">
-        <v>545.9796579621428</v>
+        <v>501.0113563579205</v>
       </c>
       <c r="H125" t="n">
-        <v>1109.457838969915</v>
+        <v>1361.339800239773</v>
       </c>
       <c r="I125" t="n">
-        <v>580.2989723736275</v>
+        <v>548.4967803065897</v>
       </c>
       <c r="J125" t="n">
-        <v>1109.457838969915</v>
+        <v>1361.339800239773</v>
       </c>
     </row>
     <row r="126">
@@ -5705,16 +5705,16 @@
         </is>
       </c>
       <c r="G126" t="n">
-        <v>600</v>
+        <v>452.7494219895172</v>
       </c>
       <c r="H126" t="n">
-        <v>1105.964351113453</v>
+        <v>1228.205012865985</v>
       </c>
       <c r="I126" t="n">
-        <v>671.866395981814</v>
+        <v>556.87093802574</v>
       </c>
       <c r="J126" t="n">
-        <v>1105.964351113453</v>
+        <v>1228.205012865985</v>
       </c>
     </row>
     <row r="127">
@@ -5745,16 +5745,16 @@
         </is>
       </c>
       <c r="G127" t="n">
-        <v>420</v>
+        <v>500.3502761097382</v>
       </c>
       <c r="H127" t="n">
-        <v>1283.028608352548</v>
+        <v>1088.175192682754</v>
       </c>
       <c r="I127" t="n">
-        <v>536.0847971477875</v>
+        <v>541.8067373771657</v>
       </c>
       <c r="J127" t="n">
-        <v>1283.028608352548</v>
+        <v>1088.175192682754</v>
       </c>
     </row>
     <row r="128">
@@ -5785,16 +5785,16 @@
         </is>
       </c>
       <c r="G128" t="n">
-        <v>561.6805206327014</v>
+        <v>433.2248705772892</v>
       </c>
       <c r="H128" t="n">
-        <v>1289.015083002636</v>
+        <v>1357.472342104878</v>
       </c>
       <c r="I128" t="n">
-        <v>619.2817002470579</v>
+        <v>454.3395608582073</v>
       </c>
       <c r="J128" t="n">
-        <v>1289.015083002636</v>
+        <v>1357.472342104878</v>
       </c>
     </row>
     <row r="129">
@@ -5825,16 +5825,16 @@
         </is>
       </c>
       <c r="G129" t="n">
-        <v>561.4474984827752</v>
+        <v>420</v>
       </c>
       <c r="H129" t="n">
-        <v>1111.327319160205</v>
+        <v>1106.718916643896</v>
       </c>
       <c r="I129" t="n">
-        <v>681.4474984827752</v>
+        <v>441.1381089720581</v>
       </c>
       <c r="J129" t="n">
-        <v>1111.327319160205</v>
+        <v>1106.718916643896</v>
       </c>
     </row>
     <row r="130">
@@ -5865,16 +5865,16 @@
         </is>
       </c>
       <c r="G130" t="n">
-        <v>489.214343723869</v>
+        <v>564.9598491021552</v>
       </c>
       <c r="H130" t="n">
-        <v>1020</v>
+        <v>1185.9067934179</v>
       </c>
       <c r="I130" t="n">
-        <v>544.3497935202786</v>
+        <v>616.498809016666</v>
       </c>
       <c r="J130" t="n">
-        <v>1020</v>
+        <v>1185.9067934179</v>
       </c>
     </row>
     <row r="131">
@@ -5905,16 +5905,16 @@
         </is>
       </c>
       <c r="G131" t="n">
-        <v>451.8823339391292</v>
+        <v>420</v>
       </c>
       <c r="H131" t="n">
-        <v>1440</v>
+        <v>1234.25133897974</v>
       </c>
       <c r="I131" t="n">
-        <v>539.3071722517403</v>
+        <v>478.6460778569243</v>
       </c>
       <c r="J131" t="n">
-        <v>1440</v>
+        <v>1234.25133897974</v>
       </c>
     </row>
     <row r="132">
@@ -5945,16 +5945,16 @@
         </is>
       </c>
       <c r="G132" t="n">
-        <v>420</v>
+        <v>484.8656698197467</v>
       </c>
       <c r="H132" t="n">
-        <v>1020</v>
+        <v>1440</v>
       </c>
       <c r="I132" t="n">
-        <v>474.4437901417584</v>
+        <v>591.8944223918481</v>
       </c>
       <c r="J132" t="n">
-        <v>1020</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="133">
@@ -5985,16 +5985,16 @@
         </is>
       </c>
       <c r="G133" t="n">
-        <v>495.7127632259537</v>
+        <v>529.4497494539961</v>
       </c>
       <c r="H133" t="n">
-        <v>1062.999190022026</v>
+        <v>1020</v>
       </c>
       <c r="I133" t="n">
-        <v>600.9978169400874</v>
+        <v>562.3319708985611</v>
       </c>
       <c r="J133" t="n">
-        <v>1062.999190022026</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="134">
@@ -6025,16 +6025,16 @@
         </is>
       </c>
       <c r="G134" t="n">
-        <v>524.7829459221221</v>
+        <v>494.4037496315186</v>
       </c>
       <c r="H134" t="n">
-        <v>1273.026230496827</v>
+        <v>1232.485709621986</v>
       </c>
       <c r="I134" t="n">
-        <v>618.1743633666279</v>
+        <v>542.0973269901516</v>
       </c>
       <c r="J134" t="n">
-        <v>1273.026230496827</v>
+        <v>1232.485709621986</v>
       </c>
     </row>
     <row r="135">
@@ -6065,16 +6065,16 @@
         </is>
       </c>
       <c r="G135" t="n">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="H135" t="n">
-        <v>1082.405197088033</v>
+        <v>1020</v>
       </c>
       <c r="I135" t="n">
-        <v>513.8073441104802</v>
+        <v>680.9282629757315</v>
       </c>
       <c r="J135" t="n">
-        <v>1082.405197088033</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="136">
@@ -6105,16 +6105,16 @@
         </is>
       </c>
       <c r="G136" t="n">
-        <v>420</v>
+        <v>508.1909484341273</v>
       </c>
       <c r="H136" t="n">
-        <v>1183.650234987851</v>
+        <v>1182.117924882775</v>
       </c>
       <c r="I136" t="n">
-        <v>521.2062041810334</v>
+        <v>600.0825545944111</v>
       </c>
       <c r="J136" t="n">
-        <v>1183.650234987851</v>
+        <v>1182.117924882775</v>
       </c>
     </row>
     <row r="137">
@@ -6145,16 +6145,16 @@
         </is>
       </c>
       <c r="G137" t="n">
-        <v>514.8950348895411</v>
+        <v>447.9805805162744</v>
       </c>
       <c r="H137" t="n">
-        <v>1069.90401873704</v>
+        <v>1225.747141798899</v>
       </c>
       <c r="I137" t="n">
-        <v>608.1134513864199</v>
+        <v>557.9935541694105</v>
       </c>
       <c r="J137" t="n">
-        <v>1069.90401873704</v>
+        <v>1225.747141798899</v>
       </c>
     </row>
     <row r="138">
@@ -6185,16 +6185,16 @@
         </is>
       </c>
       <c r="G138" t="n">
-        <v>435.1648833916811</v>
+        <v>428.1070801019502</v>
       </c>
       <c r="H138" t="n">
-        <v>1020</v>
+        <v>1148.825674358548</v>
       </c>
       <c r="I138" t="n">
-        <v>499.5032869275577</v>
+        <v>522.5810078542484</v>
       </c>
       <c r="J138" t="n">
-        <v>1020</v>
+        <v>1148.825674358548</v>
       </c>
     </row>
     <row r="139">
@@ -6225,16 +6225,16 @@
         </is>
       </c>
       <c r="G139" t="n">
-        <v>426.0288463863378</v>
+        <v>458.3694422257848</v>
       </c>
       <c r="H139" t="n">
-        <v>1347.97669817047</v>
+        <v>1202.871584028376</v>
       </c>
       <c r="I139" t="n">
-        <v>519.3136118903312</v>
+        <v>578.3694422257848</v>
       </c>
       <c r="J139" t="n">
-        <v>1347.97669817047</v>
+        <v>1202.871584028376</v>
       </c>
     </row>
     <row r="140">
@@ -6265,16 +6265,16 @@
         </is>
       </c>
       <c r="G140" t="n">
-        <v>574.6646867831811</v>
+        <v>420</v>
       </c>
       <c r="H140" t="n">
-        <v>1109.726300288736</v>
+        <v>1192.953875904998</v>
       </c>
       <c r="I140" t="n">
-        <v>613.363596285363</v>
+        <v>475.8662244922655</v>
       </c>
       <c r="J140" t="n">
-        <v>1109.726300288736</v>
+        <v>1192.953875904998</v>
       </c>
     </row>
     <row r="141">
@@ -6305,16 +6305,16 @@
         </is>
       </c>
       <c r="G141" t="n">
-        <v>546.3060444991511</v>
+        <v>422.7999359151198</v>
       </c>
       <c r="H141" t="n">
-        <v>1020</v>
+        <v>1166.677484088443</v>
       </c>
       <c r="I141" t="n">
-        <v>599.4456272555241</v>
+        <v>502.839199131308</v>
       </c>
       <c r="J141" t="n">
-        <v>1020</v>
+        <v>1166.677484088443</v>
       </c>
     </row>
     <row r="142">
@@ -6345,16 +6345,16 @@
         </is>
       </c>
       <c r="G142" t="n">
-        <v>420</v>
+        <v>524.1549717092756</v>
       </c>
       <c r="H142" t="n">
-        <v>1081.24157640615</v>
+        <v>1187.863798660333</v>
       </c>
       <c r="I142" t="n">
-        <v>479.9776314163719</v>
+        <v>583.2033932209786</v>
       </c>
       <c r="J142" t="n">
-        <v>1081.24157640615</v>
+        <v>1187.863798660333</v>
       </c>
     </row>
     <row r="143">
@@ -6385,16 +6385,16 @@
         </is>
       </c>
       <c r="G143" t="n">
-        <v>499.2071899224691</v>
+        <v>557.9242487240143</v>
       </c>
       <c r="H143" t="n">
-        <v>1020</v>
+        <v>1166.295721628515</v>
       </c>
       <c r="I143" t="n">
-        <v>574.7884140227341</v>
+        <v>601.1624619553933</v>
       </c>
       <c r="J143" t="n">
-        <v>1020</v>
+        <v>1166.295721628515</v>
       </c>
     </row>
     <row r="144">
@@ -6425,16 +6425,16 @@
         </is>
       </c>
       <c r="G144" t="n">
-        <v>550.1526268788418</v>
+        <v>575.2427109133193</v>
       </c>
       <c r="H144" t="n">
-        <v>1292.706649277154</v>
+        <v>1059.607611529778</v>
       </c>
       <c r="I144" t="n">
-        <v>619.9904820781508</v>
+        <v>588.5350747265342</v>
       </c>
       <c r="J144" t="n">
-        <v>1292.706649277154</v>
+        <v>1059.607611529778</v>
       </c>
     </row>
     <row r="145">
@@ -6465,16 +6465,16 @@
         </is>
       </c>
       <c r="G145" t="n">
-        <v>535.0775339875277</v>
+        <v>484.3388156956037</v>
       </c>
       <c r="H145" t="n">
-        <v>1199.847032579228</v>
+        <v>1140.105414972975</v>
       </c>
       <c r="I145" t="n">
-        <v>535.0775339875277</v>
+        <v>529.9534774370079</v>
       </c>
       <c r="J145" t="n">
-        <v>1199.847032579228</v>
+        <v>1140.105414972975</v>
       </c>
     </row>
     <row r="146">
@@ -6505,16 +6505,16 @@
         </is>
       </c>
       <c r="G146" t="n">
-        <v>420</v>
+        <v>517.5408444872414</v>
       </c>
       <c r="H146" t="n">
-        <v>1020</v>
+        <v>1034.04143253911</v>
       </c>
       <c r="I146" t="n">
-        <v>485.1496231879476</v>
+        <v>576.0833760894573</v>
       </c>
       <c r="J146" t="n">
-        <v>1020</v>
+        <v>1034.04143253911</v>
       </c>
     </row>
     <row r="147">
@@ -6545,16 +6545,16 @@
         </is>
       </c>
       <c r="G147" t="n">
-        <v>486.9728189322956</v>
+        <v>439.8613294626766</v>
       </c>
       <c r="H147" t="n">
-        <v>1177.499232824326</v>
+        <v>1206.24134741173</v>
       </c>
       <c r="I147" t="n">
-        <v>486.9728189322956</v>
+        <v>519.9702086497109</v>
       </c>
       <c r="J147" t="n">
-        <v>1177.499232824326</v>
+        <v>1206.24134741173</v>
       </c>
     </row>
     <row r="148">
@@ -6585,16 +6585,16 @@
         </is>
       </c>
       <c r="G148" t="n">
-        <v>456.1897553837919</v>
+        <v>490.0098256600764</v>
       </c>
       <c r="H148" t="n">
-        <v>1055.255631720638</v>
+        <v>1163.930328364201</v>
       </c>
       <c r="I148" t="n">
-        <v>526.2426223702109</v>
+        <v>551.5606672626534</v>
       </c>
       <c r="J148" t="n">
-        <v>1055.255631720638</v>
+        <v>1163.930328364201</v>
       </c>
     </row>
     <row r="149">
@@ -6625,16 +6625,16 @@
         </is>
       </c>
       <c r="G149" t="n">
-        <v>475.3376320557522</v>
+        <v>505.4870087667195</v>
       </c>
       <c r="H149" t="n">
-        <v>1020</v>
+        <v>1032.46309197824</v>
       </c>
       <c r="I149" t="n">
-        <v>534.5389244156171</v>
+        <v>522.3934153444504</v>
       </c>
       <c r="J149" t="n">
-        <v>1020</v>
+        <v>1032.46309197824</v>
       </c>
     </row>
     <row r="150">
@@ -6665,16 +6665,16 @@
         </is>
       </c>
       <c r="G150" t="n">
-        <v>474.4756210512872</v>
+        <v>600</v>
       </c>
       <c r="H150" t="n">
-        <v>1124.347970657587</v>
+        <v>1205.776308423441</v>
       </c>
       <c r="I150" t="n">
-        <v>537.908422352717</v>
+        <v>651.8310019619182</v>
       </c>
       <c r="J150" t="n">
-        <v>1124.347970657587</v>
+        <v>1205.776308423441</v>
       </c>
     </row>
     <row r="151">
@@ -6705,16 +6705,16 @@
         </is>
       </c>
       <c r="G151" t="n">
-        <v>435.9434924279632</v>
+        <v>486.0541190806748</v>
       </c>
       <c r="H151" t="n">
-        <v>1020</v>
+        <v>1351.239292539237</v>
       </c>
       <c r="I151" t="n">
-        <v>524.7455411925646</v>
+        <v>539.4918152274512</v>
       </c>
       <c r="J151" t="n">
-        <v>1020</v>
+        <v>1351.239292539237</v>
       </c>
     </row>
     <row r="152">
@@ -6745,16 +6745,16 @@
         </is>
       </c>
       <c r="G152" t="n">
-        <v>420</v>
+        <v>465.7304715918485</v>
       </c>
       <c r="H152" t="n">
-        <v>1127.559340954628</v>
+        <v>1274.838903459025</v>
       </c>
       <c r="I152" t="n">
-        <v>468.1717742308294</v>
+        <v>530.7679749950695</v>
       </c>
       <c r="J152" t="n">
-        <v>1127.559340954628</v>
+        <v>1274.838903459025</v>
       </c>
     </row>
     <row r="153">
@@ -6785,16 +6785,16 @@
         </is>
       </c>
       <c r="G153" t="n">
-        <v>420</v>
+        <v>600</v>
       </c>
       <c r="H153" t="n">
-        <v>1440</v>
+        <v>1108.345122190521</v>
       </c>
       <c r="I153" t="n">
-        <v>444.7155730044173</v>
+        <v>700.3298120336724</v>
       </c>
       <c r="J153" t="n">
-        <v>1440</v>
+        <v>1108.345122190521</v>
       </c>
     </row>
     <row r="154">
@@ -6825,16 +6825,16 @@
         </is>
       </c>
       <c r="G154" t="n">
-        <v>469.2397680870668</v>
+        <v>511.0484298012521</v>
       </c>
       <c r="H154" t="n">
-        <v>1020</v>
+        <v>1131.429989559836</v>
       </c>
       <c r="I154" t="n">
-        <v>492.4054222634697</v>
+        <v>544.9246691858459</v>
       </c>
       <c r="J154" t="n">
-        <v>1020</v>
+        <v>1131.429989559836</v>
       </c>
     </row>
     <row r="155">
@@ -6865,16 +6865,16 @@
         </is>
       </c>
       <c r="G155" t="n">
-        <v>420</v>
+        <v>550.9638433980426</v>
       </c>
       <c r="H155" t="n">
-        <v>1077.325354392926</v>
+        <v>1182.115571819252</v>
       </c>
       <c r="I155" t="n">
-        <v>486.15424433947</v>
+        <v>655.8225631174162</v>
       </c>
       <c r="J155" t="n">
-        <v>1077.325354392926</v>
+        <v>1182.115571819252</v>
       </c>
     </row>
     <row r="156">
@@ -6905,16 +6905,16 @@
         </is>
       </c>
       <c r="G156" t="n">
-        <v>440.4012502040136</v>
+        <v>426.215971810165</v>
       </c>
       <c r="H156" t="n">
-        <v>1075.743543200158</v>
+        <v>1020</v>
       </c>
       <c r="I156" t="n">
-        <v>504.9564076335203</v>
+        <v>512.5028127818332</v>
       </c>
       <c r="J156" t="n">
-        <v>1075.743543200158</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="157">
@@ -6945,16 +6945,16 @@
         </is>
       </c>
       <c r="G157" t="n">
-        <v>486.6506821135832</v>
+        <v>420</v>
       </c>
       <c r="H157" t="n">
-        <v>1109.889860854923</v>
+        <v>1160.417605505792</v>
       </c>
       <c r="I157" t="n">
-        <v>528.7217368249323</v>
+        <v>486.0368033959065</v>
       </c>
       <c r="J157" t="n">
-        <v>1109.889860854923</v>
+        <v>1160.417605505792</v>
       </c>
     </row>
     <row r="158">
@@ -6985,16 +6985,16 @@
         </is>
       </c>
       <c r="G158" t="n">
-        <v>574.5838486280976</v>
+        <v>516.9568649756609</v>
       </c>
       <c r="H158" t="n">
-        <v>1020</v>
+        <v>1102.938616949756</v>
       </c>
       <c r="I158" t="n">
-        <v>639.8240985048616</v>
+        <v>604.1519443339287</v>
       </c>
       <c r="J158" t="n">
-        <v>1020</v>
+        <v>1102.938616949756</v>
       </c>
     </row>
     <row r="159">
@@ -7025,16 +7025,16 @@
         </is>
       </c>
       <c r="G159" t="n">
-        <v>534.3856014454939</v>
+        <v>465.342728502158</v>
       </c>
       <c r="H159" t="n">
-        <v>1231.861474936166</v>
+        <v>1020</v>
       </c>
       <c r="I159" t="n">
-        <v>581.4741116311296</v>
+        <v>523.89242224625</v>
       </c>
       <c r="J159" t="n">
-        <v>1231.861474936166</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="160">
@@ -7065,16 +7065,16 @@
         </is>
       </c>
       <c r="G160" t="n">
-        <v>472.0985691448534</v>
+        <v>520.0085985142947</v>
       </c>
       <c r="H160" t="n">
-        <v>1020</v>
+        <v>1166.480686715284</v>
       </c>
       <c r="I160" t="n">
-        <v>525.0686745511003</v>
+        <v>586.9616675152278</v>
       </c>
       <c r="J160" t="n">
-        <v>1020</v>
+        <v>1166.480686715284</v>
       </c>
     </row>
     <row r="161">
@@ -7105,16 +7105,16 @@
         </is>
       </c>
       <c r="G161" t="n">
-        <v>468.0979982391904</v>
+        <v>420</v>
       </c>
       <c r="H161" t="n">
-        <v>1222.532992730108</v>
+        <v>1177.840993064951</v>
       </c>
       <c r="I161" t="n">
-        <v>521.4554498340631</v>
+        <v>463.5311082283753</v>
       </c>
       <c r="J161" t="n">
-        <v>1222.532992730108</v>
+        <v>1177.840993064951</v>
       </c>
     </row>
     <row r="162">
@@ -7145,16 +7145,16 @@
         </is>
       </c>
       <c r="G162" t="n">
-        <v>517.0604198432769</v>
+        <v>561.8551207687503</v>
       </c>
       <c r="H162" t="n">
-        <v>1022.140714946272</v>
+        <v>1138.645789666388</v>
       </c>
       <c r="I162" t="n">
-        <v>577.0206472365138</v>
+        <v>628.722614577377</v>
       </c>
       <c r="J162" t="n">
-        <v>1022.140714946272</v>
+        <v>1138.645789666388</v>
       </c>
     </row>
     <row r="163">
@@ -7185,13 +7185,13 @@
         </is>
       </c>
       <c r="G163" t="n">
-        <v>438.9903045826759</v>
+        <v>422.2346698260536</v>
       </c>
       <c r="H163" t="n">
         <v>1020</v>
       </c>
       <c r="I163" t="n">
-        <v>462.3115331355198</v>
+        <v>510.0581326000214</v>
       </c>
       <c r="J163" t="n">
         <v>1020</v>
@@ -7225,16 +7225,16 @@
         </is>
       </c>
       <c r="G164" t="n">
-        <v>470.7876176319224</v>
+        <v>600</v>
       </c>
       <c r="H164" t="n">
-        <v>1440</v>
+        <v>1047.571854820889</v>
       </c>
       <c r="I164" t="n">
-        <v>566.0506018124145</v>
+        <v>652.1316632103566</v>
       </c>
       <c r="J164" t="n">
-        <v>1440</v>
+        <v>1047.571854820889</v>
       </c>
     </row>
     <row r="165">
@@ -7265,16 +7265,16 @@
         </is>
       </c>
       <c r="G165" t="n">
-        <v>420</v>
+        <v>505.5608382916039</v>
       </c>
       <c r="H165" t="n">
-        <v>1020</v>
+        <v>1068.072103121416</v>
       </c>
       <c r="I165" t="n">
-        <v>499.2235249197686</v>
+        <v>552.8380995256111</v>
       </c>
       <c r="J165" t="n">
-        <v>1020</v>
+        <v>1068.072103121416</v>
       </c>
     </row>
     <row r="166">
@@ -7305,16 +7305,16 @@
         </is>
       </c>
       <c r="G166" t="n">
-        <v>557.7959613509991</v>
+        <v>551.1162435822962</v>
       </c>
       <c r="H166" t="n">
-        <v>1141.153212471629</v>
+        <v>1182.973254608258</v>
       </c>
       <c r="I166" t="n">
-        <v>616.2266539323323</v>
+        <v>621.9197952963221</v>
       </c>
       <c r="J166" t="n">
-        <v>1141.153212471629</v>
+        <v>1182.973254608258</v>
       </c>
     </row>
     <row r="167">
@@ -7345,16 +7345,16 @@
         </is>
       </c>
       <c r="G167" t="n">
-        <v>519.1497710615379</v>
+        <v>528.9823854707773</v>
       </c>
       <c r="H167" t="n">
-        <v>1149.334374583765</v>
+        <v>1020</v>
       </c>
       <c r="I167" t="n">
-        <v>611.6745746134638</v>
+        <v>638.6340454221466</v>
       </c>
       <c r="J167" t="n">
-        <v>1149.334374583765</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="168">
@@ -7385,16 +7385,16 @@
         </is>
       </c>
       <c r="G168" t="n">
-        <v>440.0125405762601</v>
+        <v>516.0618460390162</v>
       </c>
       <c r="H168" t="n">
-        <v>1220.327928643376</v>
+        <v>1432.288828396103</v>
       </c>
       <c r="I168" t="n">
-        <v>471.7776345095041</v>
+        <v>516.0618460390162</v>
       </c>
       <c r="J168" t="n">
-        <v>1220.327928643376</v>
+        <v>1432.288828396103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
integration of both init and togo
now it works (yeeeaah)
</commit_message>
<xml_diff>
--- a/data/Otxarkoaga/population/pop_building.xlsx
+++ b/data/Otxarkoaga/population/pop_building.xlsx
@@ -509,7 +509,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G2" t="n">
@@ -553,7 +553,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G3" t="n">
@@ -597,7 +597,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G4" t="n">
@@ -641,7 +641,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G5" t="n">
@@ -685,7 +685,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G6" t="n">
@@ -729,7 +729,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G7" t="n">
@@ -773,7 +773,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G8" t="n">
@@ -817,7 +817,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G9" t="n">
@@ -861,7 +861,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G10" t="n">
@@ -905,7 +905,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G11" t="n">
@@ -949,7 +949,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G12" t="n">
@@ -993,7 +993,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G13" t="n">
@@ -1037,7 +1037,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G14" t="n">
@@ -1081,7 +1081,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G15" t="n">
@@ -1125,7 +1125,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G16" t="n">
@@ -1169,7 +1169,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G17" t="n">
@@ -1213,7 +1213,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G18" t="n">
@@ -1257,7 +1257,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G19" t="n">
@@ -1301,7 +1301,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G20" t="n">
@@ -1345,7 +1345,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G21" t="n">
@@ -1389,7 +1389,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G22" t="n">
@@ -1433,7 +1433,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G23" t="n">
@@ -1477,7 +1477,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G24" t="n">
@@ -1521,7 +1521,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G25" t="n">
@@ -1565,7 +1565,7 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G26" t="n">
@@ -1609,7 +1609,7 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G27" t="n">
@@ -1653,7 +1653,7 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G28" t="n">
@@ -1697,7 +1697,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G29" t="n">
@@ -1741,7 +1741,7 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G30" t="n">
@@ -1785,7 +1785,7 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G31" t="n">
@@ -1829,7 +1829,7 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G32" t="n">
@@ -1873,7 +1873,7 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G33" t="n">
@@ -1917,7 +1917,7 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G34" t="n">
@@ -1961,7 +1961,7 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G35" t="n">
@@ -2005,7 +2005,7 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G36" t="n">
@@ -2049,7 +2049,7 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G37" t="n">
@@ -2093,7 +2093,7 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G38" t="n">
@@ -2137,7 +2137,7 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G39" t="n">
@@ -2181,7 +2181,7 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G40" t="n">
@@ -2225,7 +2225,7 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G41" t="n">
@@ -2269,7 +2269,7 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G42" t="n">
@@ -2313,7 +2313,7 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G43" t="n">
@@ -2357,7 +2357,7 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G44" t="n">
@@ -2401,7 +2401,7 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G45" t="n">
@@ -2445,7 +2445,7 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G46" t="n">
@@ -2489,7 +2489,7 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G47" t="n">
@@ -2533,7 +2533,7 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G48" t="n">
@@ -2577,7 +2577,7 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G49" t="n">
@@ -2621,7 +2621,7 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G50" t="n">
@@ -2665,7 +2665,7 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G51" t="n">
@@ -2709,7 +2709,7 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G52" t="n">
@@ -2753,7 +2753,7 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G53" t="n">
@@ -2797,7 +2797,7 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G54" t="n">
@@ -2841,7 +2841,7 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G55" t="n">
@@ -2885,7 +2885,7 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G56" t="n">
@@ -2929,7 +2929,7 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G57" t="n">
@@ -2973,7 +2973,7 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G58" t="n">
@@ -3017,7 +3017,7 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>Home</t>
         </is>
       </c>
       <c r="G59" t="n">
@@ -3065,16 +3065,16 @@
         </is>
       </c>
       <c r="G60" t="n">
-        <v>425.6199974785681</v>
+        <v>467.567377743479</v>
       </c>
       <c r="H60" t="n">
-        <v>1109.81909692339</v>
+        <v>1061.46530917929</v>
       </c>
       <c r="I60" t="n">
-        <v>488.7549500135832</v>
+        <v>535.7320908257171</v>
       </c>
       <c r="J60" t="n">
-        <v>1109.81909692339</v>
+        <v>1061.46530917929</v>
       </c>
     </row>
     <row r="61">
@@ -3105,16 +3105,16 @@
         </is>
       </c>
       <c r="G61" t="n">
-        <v>484.3341223874794</v>
+        <v>479.6099721943433</v>
       </c>
       <c r="H61" t="n">
-        <v>1060</v>
+        <v>1096.778605181335</v>
       </c>
       <c r="I61" t="n">
-        <v>530.2982239905306</v>
+        <v>544.9710418549079</v>
       </c>
       <c r="J61" t="n">
-        <v>1060</v>
+        <v>1096.778605181335</v>
       </c>
     </row>
     <row r="62">
@@ -3145,16 +3145,16 @@
         </is>
       </c>
       <c r="G62" t="n">
-        <v>441.4392373202759</v>
+        <v>494.2616259093687</v>
       </c>
       <c r="H62" t="n">
-        <v>1060</v>
+        <v>1106.868353160796</v>
       </c>
       <c r="I62" t="n">
-        <v>541.7930332231717</v>
+        <v>509.9175385296567</v>
       </c>
       <c r="J62" t="n">
-        <v>1060</v>
+        <v>1106.868353160796</v>
       </c>
     </row>
     <row r="63">
@@ -3185,16 +3185,16 @@
         </is>
       </c>
       <c r="G63" t="n">
-        <v>452.1935299360994</v>
+        <v>420</v>
       </c>
       <c r="H63" t="n">
-        <v>1061.545585087516</v>
+        <v>1060</v>
       </c>
       <c r="I63" t="n">
-        <v>502.6308710596613</v>
+        <v>481.0788254263013</v>
       </c>
       <c r="J63" t="n">
-        <v>1061.545585087516</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="64">
@@ -3225,16 +3225,16 @@
         </is>
       </c>
       <c r="G64" t="n">
-        <v>420</v>
+        <v>445.7365464117268</v>
       </c>
       <c r="H64" t="n">
-        <v>1131.922984461146</v>
+        <v>1066.395960264228</v>
       </c>
       <c r="I64" t="n">
-        <v>456.3772072549711</v>
+        <v>508.5582616768806</v>
       </c>
       <c r="J64" t="n">
-        <v>1131.922984461146</v>
+        <v>1066.395960264228</v>
       </c>
     </row>
     <row r="65">
@@ -3265,16 +3265,16 @@
         </is>
       </c>
       <c r="G65" t="n">
-        <v>486.7059351889586</v>
+        <v>431.8653593708257</v>
       </c>
       <c r="H65" t="n">
-        <v>1060</v>
+        <v>1098.046699028888</v>
       </c>
       <c r="I65" t="n">
-        <v>562.0362784977859</v>
+        <v>509.4798003861916</v>
       </c>
       <c r="J65" t="n">
-        <v>1060</v>
+        <v>1098.046699028888</v>
       </c>
     </row>
     <row r="66">
@@ -3305,16 +3305,16 @@
         </is>
       </c>
       <c r="G66" t="n">
-        <v>448.7945382386145</v>
+        <v>427.9581927482965</v>
       </c>
       <c r="H66" t="n">
-        <v>1093.034705620703</v>
+        <v>1071.475332185788</v>
       </c>
       <c r="I66" t="n">
-        <v>458.8722132280118</v>
+        <v>512.3642555204162</v>
       </c>
       <c r="J66" t="n">
-        <v>1093.034705620703</v>
+        <v>1071.475332185788</v>
       </c>
     </row>
     <row r="67">
@@ -3345,16 +3345,16 @@
         </is>
       </c>
       <c r="G67" t="n">
-        <v>474.5854885093802</v>
+        <v>437.5698390131587</v>
       </c>
       <c r="H67" t="n">
-        <v>1102.418640316122</v>
+        <v>1071.366597981245</v>
       </c>
       <c r="I67" t="n">
-        <v>493.6266222359977</v>
+        <v>517.9739457380202</v>
       </c>
       <c r="J67" t="n">
-        <v>1102.418640316122</v>
+        <v>1071.366597981245</v>
       </c>
     </row>
     <row r="68">
@@ -3385,16 +3385,16 @@
         </is>
       </c>
       <c r="G68" t="n">
-        <v>440.5405962937811</v>
+        <v>420.9557936520869</v>
       </c>
       <c r="H68" t="n">
-        <v>1086.113437186111</v>
+        <v>1082.493447276799</v>
       </c>
       <c r="I68" t="n">
-        <v>541.3548569860993</v>
+        <v>473.0598748156573</v>
       </c>
       <c r="J68" t="n">
-        <v>1086.113437186111</v>
+        <v>1082.493447276799</v>
       </c>
     </row>
     <row r="69">
@@ -3421,20 +3421,20 @@
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>dutties</t>
+          <t>Dutties</t>
         </is>
       </c>
       <c r="G69" t="n">
-        <v>461.1170142547982</v>
+        <v>492.6735418210682</v>
       </c>
       <c r="H69" t="n">
-        <v>1281.308066815435</v>
+        <v>1305.307786556421</v>
       </c>
       <c r="I69" t="n">
-        <v>468.6150451318845</v>
+        <v>612.6735418210682</v>
       </c>
       <c r="J69" t="n">
-        <v>1281.308066815435</v>
+        <v>1305.307786556421</v>
       </c>
     </row>
     <row r="70">
@@ -3461,20 +3461,20 @@
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>dutties</t>
+          <t>Dutties</t>
         </is>
       </c>
       <c r="G70" t="n">
-        <v>525.8686705755246</v>
+        <v>482.4639686696427</v>
       </c>
       <c r="H70" t="n">
-        <v>1176.413156887814</v>
+        <v>1237.388145570786</v>
       </c>
       <c r="I70" t="n">
-        <v>570.0616721818711</v>
+        <v>574.938014776758</v>
       </c>
       <c r="J70" t="n">
-        <v>1176.413156887814</v>
+        <v>1237.388145570786</v>
       </c>
     </row>
     <row r="71">
@@ -3501,20 +3501,20 @@
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>dutties</t>
+          <t>Dutties</t>
         </is>
       </c>
       <c r="G71" t="n">
-        <v>517.8981423842758</v>
+        <v>505.6048888679616</v>
       </c>
       <c r="H71" t="n">
-        <v>1282.994780038358</v>
+        <v>1218.319984164578</v>
       </c>
       <c r="I71" t="n">
-        <v>581.2803879100582</v>
+        <v>592.9288202449025</v>
       </c>
       <c r="J71" t="n">
-        <v>1282.994780038358</v>
+        <v>1218.319984164578</v>
       </c>
     </row>
     <row r="72">
@@ -3541,20 +3541,20 @@
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>dutties</t>
+          <t>Dutties</t>
         </is>
       </c>
       <c r="G72" t="n">
-        <v>492.5022711832751</v>
+        <v>540</v>
       </c>
       <c r="H72" t="n">
-        <v>1320</v>
+        <v>1295.776710407343</v>
       </c>
       <c r="I72" t="n">
-        <v>593.4539102557748</v>
+        <v>615.5420018208891</v>
       </c>
       <c r="J72" t="n">
-        <v>1320</v>
+        <v>1295.776710407343</v>
       </c>
     </row>
     <row r="73">
@@ -3581,20 +3581,20 @@
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>dutties</t>
+          <t>Dutties</t>
         </is>
       </c>
       <c r="G73" t="n">
-        <v>500.4678341046388</v>
+        <v>478.9961194438843</v>
       </c>
       <c r="H73" t="n">
-        <v>1224.181282280326</v>
+        <v>1197.839366242365</v>
       </c>
       <c r="I73" t="n">
-        <v>553.5753285438309</v>
+        <v>598.9961194438843</v>
       </c>
       <c r="J73" t="n">
-        <v>1224.181282280326</v>
+        <v>1197.839366242365</v>
       </c>
     </row>
     <row r="74">
@@ -3621,20 +3621,20 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>dutties</t>
+          <t>Dutties</t>
         </is>
       </c>
       <c r="G74" t="n">
-        <v>434.2955056022997</v>
+        <v>429.0356878007408</v>
       </c>
       <c r="H74" t="n">
-        <v>1269.503486543706</v>
+        <v>1320</v>
       </c>
       <c r="I74" t="n">
-        <v>545.7078446187787</v>
+        <v>458.9777447436769</v>
       </c>
       <c r="J74" t="n">
-        <v>1269.503486543706</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="75">
@@ -3661,20 +3661,20 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>dutties</t>
+          <t>Dutties</t>
         </is>
       </c>
       <c r="G75" t="n">
-        <v>474.0308815501552</v>
+        <v>463.3305797044458</v>
       </c>
       <c r="H75" t="n">
-        <v>1230.552887388359</v>
+        <v>1258.244240214454</v>
       </c>
       <c r="I75" t="n">
-        <v>527.8663272849549</v>
+        <v>541.2550725580427</v>
       </c>
       <c r="J75" t="n">
-        <v>1230.552887388359</v>
+        <v>1258.244240214454</v>
       </c>
     </row>
     <row r="76">
@@ -3701,20 +3701,20 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>dutties</t>
+          <t>Dutties</t>
         </is>
       </c>
       <c r="G76" t="n">
         <v>540</v>
       </c>
       <c r="H76" t="n">
-        <v>1286.785940718925</v>
+        <v>1288.33671924836</v>
       </c>
       <c r="I76" t="n">
-        <v>660</v>
+        <v>602.5114339586444</v>
       </c>
       <c r="J76" t="n">
-        <v>1286.785940718925</v>
+        <v>1288.33671924836</v>
       </c>
     </row>
     <row r="77">
@@ -3741,20 +3741,20 @@
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>dutties</t>
+          <t>Dutties</t>
         </is>
       </c>
       <c r="G77" t="n">
-        <v>428.1153792110128</v>
+        <v>465.759145229928</v>
       </c>
       <c r="H77" t="n">
-        <v>1320</v>
+        <v>1164.503976354888</v>
       </c>
       <c r="I77" t="n">
-        <v>481.3229063003999</v>
+        <v>529.0272254186282</v>
       </c>
       <c r="J77" t="n">
-        <v>1320</v>
+        <v>1164.503976354888</v>
       </c>
     </row>
     <row r="78">
@@ -3781,20 +3781,20 @@
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>dutties</t>
+          <t>Dutties</t>
         </is>
       </c>
       <c r="G78" t="n">
-        <v>434.9680898387795</v>
+        <v>495.8436524121105</v>
       </c>
       <c r="H78" t="n">
-        <v>1272.531443361663</v>
+        <v>1228.074831254891</v>
       </c>
       <c r="I78" t="n">
-        <v>513.5164476963356</v>
+        <v>521.4344322339994</v>
       </c>
       <c r="J78" t="n">
-        <v>1272.531443361663</v>
+        <v>1228.074831254891</v>
       </c>
     </row>
     <row r="79">
@@ -3821,20 +3821,20 @@
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>dutties</t>
+          <t>Dutties</t>
         </is>
       </c>
       <c r="G79" t="n">
-        <v>429.8896967555555</v>
+        <v>421.1708829629714</v>
       </c>
       <c r="H79" t="n">
-        <v>1320</v>
+        <v>1310.062140626584</v>
       </c>
       <c r="I79" t="n">
-        <v>521.6389061639875</v>
+        <v>490.206054773554</v>
       </c>
       <c r="J79" t="n">
-        <v>1320</v>
+        <v>1310.062140626584</v>
       </c>
     </row>
     <row r="80">
@@ -3861,20 +3861,20 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>dutties</t>
+          <t>Dutties</t>
         </is>
       </c>
       <c r="G80" t="n">
-        <v>494.656747729738</v>
+        <v>459.6867014707641</v>
       </c>
       <c r="H80" t="n">
-        <v>1320</v>
+        <v>1290.044209452009</v>
       </c>
       <c r="I80" t="n">
-        <v>562.2589866162052</v>
+        <v>504.5831746823475</v>
       </c>
       <c r="J80" t="n">
-        <v>1320</v>
+        <v>1290.044209452009</v>
       </c>
     </row>
     <row r="81">
@@ -3901,20 +3901,20 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>dutties</t>
+          <t>Dutties</t>
         </is>
       </c>
       <c r="G81" t="n">
-        <v>466.8235572255791</v>
+        <v>526.0088973773717</v>
       </c>
       <c r="H81" t="n">
-        <v>1193.154541366167</v>
+        <v>1244.875744505704</v>
       </c>
       <c r="I81" t="n">
-        <v>468.1118237558955</v>
+        <v>579.2575891370143</v>
       </c>
       <c r="J81" t="n">
-        <v>1193.154541366167</v>
+        <v>1244.875744505704</v>
       </c>
     </row>
     <row r="82">
@@ -3945,16 +3945,16 @@
         </is>
       </c>
       <c r="G82" t="n">
-        <v>488.7652522169874</v>
+        <v>480.3203772187004</v>
       </c>
       <c r="H82" t="n">
-        <v>1133.320286013789</v>
+        <v>1320</v>
       </c>
       <c r="I82" t="n">
-        <v>488.7652522169874</v>
+        <v>480.3203772187004</v>
       </c>
       <c r="J82" t="n">
-        <v>1133.320286013789</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="83">
@@ -3985,16 +3985,16 @@
         </is>
       </c>
       <c r="G83" t="n">
-        <v>520.5417811676833</v>
+        <v>483.8436462352041</v>
       </c>
       <c r="H83" t="n">
-        <v>1236.225079544521</v>
+        <v>1239.096474493268</v>
       </c>
       <c r="I83" t="n">
-        <v>520.5417811676833</v>
+        <v>483.8436462352041</v>
       </c>
       <c r="J83" t="n">
-        <v>1236.225079544521</v>
+        <v>1239.096474493268</v>
       </c>
     </row>
     <row r="84">
@@ -4025,16 +4025,16 @@
         </is>
       </c>
       <c r="G84" t="n">
-        <v>498.759920070242</v>
+        <v>540</v>
       </c>
       <c r="H84" t="n">
-        <v>1314.659401594806</v>
+        <v>1056.57452052503</v>
       </c>
       <c r="I84" t="n">
-        <v>498.759920070242</v>
+        <v>540</v>
       </c>
       <c r="J84" t="n">
-        <v>1314.659401594806</v>
+        <v>1056.57452052503</v>
       </c>
     </row>
     <row r="85">
@@ -4065,16 +4065,16 @@
         </is>
       </c>
       <c r="G85" t="n">
-        <v>492.8863058849175</v>
+        <v>493.4028692363369</v>
       </c>
       <c r="H85" t="n">
-        <v>1250.535866987504</v>
+        <v>1148.112385296805</v>
       </c>
       <c r="I85" t="n">
-        <v>492.8863058849175</v>
+        <v>493.4028692363369</v>
       </c>
       <c r="J85" t="n">
-        <v>1250.535866987504</v>
+        <v>1148.112385296805</v>
       </c>
     </row>
     <row r="86">
@@ -4105,16 +4105,16 @@
         </is>
       </c>
       <c r="G86" t="n">
-        <v>473.9417294651641</v>
+        <v>477.5121603073295</v>
       </c>
       <c r="H86" t="n">
-        <v>1235.240927559497</v>
+        <v>1292.095776660803</v>
       </c>
       <c r="I86" t="n">
-        <v>473.9417294651641</v>
+        <v>477.5121603073295</v>
       </c>
       <c r="J86" t="n">
-        <v>1235.240927559497</v>
+        <v>1292.095776660803</v>
       </c>
     </row>
     <row r="87">
@@ -4145,16 +4145,16 @@
         </is>
       </c>
       <c r="G87" t="n">
-        <v>510.894816117106</v>
+        <v>472.5016104380961</v>
       </c>
       <c r="H87" t="n">
-        <v>1275.51436535502</v>
+        <v>1232.719461906569</v>
       </c>
       <c r="I87" t="n">
-        <v>510.894816117106</v>
+        <v>472.5016104380961</v>
       </c>
       <c r="J87" t="n">
-        <v>1275.51436535502</v>
+        <v>1232.719461906569</v>
       </c>
     </row>
     <row r="88">
@@ -4185,16 +4185,16 @@
         </is>
       </c>
       <c r="G88" t="n">
-        <v>530.7321297828119</v>
+        <v>444.5191788182944</v>
       </c>
       <c r="H88" t="n">
-        <v>1224.719232873604</v>
+        <v>1320</v>
       </c>
       <c r="I88" t="n">
-        <v>530.7321297828119</v>
+        <v>444.5191788182944</v>
       </c>
       <c r="J88" t="n">
-        <v>1224.719232873604</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="89">
@@ -4225,16 +4225,16 @@
         </is>
       </c>
       <c r="G89" t="n">
-        <v>540</v>
+        <v>445.7344215874504</v>
       </c>
       <c r="H89" t="n">
-        <v>1160.311147533977</v>
+        <v>1186.08148697518</v>
       </c>
       <c r="I89" t="n">
-        <v>540</v>
+        <v>445.7344215874504</v>
       </c>
       <c r="J89" t="n">
-        <v>1160.311147533977</v>
+        <v>1186.08148697518</v>
       </c>
     </row>
     <row r="90">
@@ -4265,16 +4265,16 @@
         </is>
       </c>
       <c r="G90" t="n">
-        <v>478.7276862717181</v>
+        <v>527.9370045978829</v>
       </c>
       <c r="H90" t="n">
-        <v>1250.262218651491</v>
+        <v>1151.027191672375</v>
       </c>
       <c r="I90" t="n">
-        <v>478.7276862717181</v>
+        <v>527.9370045978829</v>
       </c>
       <c r="J90" t="n">
-        <v>1250.262218651491</v>
+        <v>1151.027191672375</v>
       </c>
     </row>
     <row r="91">
@@ -4305,16 +4305,16 @@
         </is>
       </c>
       <c r="G91" t="n">
-        <v>528.5983969224268</v>
+        <v>482.0121225325758</v>
       </c>
       <c r="H91" t="n">
-        <v>1184.392696575258</v>
+        <v>1225.846590028051</v>
       </c>
       <c r="I91" t="n">
-        <v>528.5983969224268</v>
+        <v>482.0121225325758</v>
       </c>
       <c r="J91" t="n">
-        <v>1184.392696575258</v>
+        <v>1225.846590028051</v>
       </c>
     </row>
     <row r="92">
@@ -4345,16 +4345,16 @@
         </is>
       </c>
       <c r="G92" t="n">
-        <v>472.692481152121</v>
+        <v>490.9674134809853</v>
       </c>
       <c r="H92" t="n">
-        <v>1163.251296666992</v>
+        <v>1034.010568785485</v>
       </c>
       <c r="I92" t="n">
-        <v>472.692481152121</v>
+        <v>490.9674134809853</v>
       </c>
       <c r="J92" t="n">
-        <v>1163.251296666992</v>
+        <v>1034.010568785485</v>
       </c>
     </row>
     <row r="93">
@@ -4385,16 +4385,16 @@
         </is>
       </c>
       <c r="G93" t="n">
-        <v>530.0338837234964</v>
+        <v>531.5532325715832</v>
       </c>
       <c r="H93" t="n">
-        <v>1157.848153305914</v>
+        <v>1106.536211831876</v>
       </c>
       <c r="I93" t="n">
-        <v>530.0338837234964</v>
+        <v>531.5532325715832</v>
       </c>
       <c r="J93" t="n">
-        <v>1157.848153305914</v>
+        <v>1106.536211831876</v>
       </c>
     </row>
     <row r="94">
@@ -4425,16 +4425,16 @@
         </is>
       </c>
       <c r="G94" t="n">
-        <v>477.0826789483378</v>
+        <v>512.2229100117139</v>
       </c>
       <c r="H94" t="n">
-        <v>1301.259364409706</v>
+        <v>1269.794585335299</v>
       </c>
       <c r="I94" t="n">
-        <v>477.0826789483378</v>
+        <v>512.2229100117139</v>
       </c>
       <c r="J94" t="n">
-        <v>1301.259364409706</v>
+        <v>1269.794585335299</v>
       </c>
     </row>
     <row r="95">
@@ -4465,16 +4465,16 @@
         </is>
       </c>
       <c r="G95" t="n">
-        <v>505.2819891498899</v>
+        <v>478.7116868689076</v>
       </c>
       <c r="H95" t="n">
-        <v>1247.041054379891</v>
+        <v>1189.090765157907</v>
       </c>
       <c r="I95" t="n">
-        <v>505.2819891498899</v>
+        <v>478.7116868689076</v>
       </c>
       <c r="J95" t="n">
-        <v>1247.041054379891</v>
+        <v>1189.090765157907</v>
       </c>
     </row>
     <row r="96">
@@ -4505,16 +4505,16 @@
         </is>
       </c>
       <c r="G96" t="n">
-        <v>540</v>
+        <v>521.5211254070161</v>
       </c>
       <c r="H96" t="n">
-        <v>1183.091075618762</v>
+        <v>1298.770657404375</v>
       </c>
       <c r="I96" t="n">
-        <v>540</v>
+        <v>521.5211254070161</v>
       </c>
       <c r="J96" t="n">
-        <v>1183.091075618762</v>
+        <v>1298.770657404375</v>
       </c>
     </row>
     <row r="97">
@@ -4545,16 +4545,16 @@
         </is>
       </c>
       <c r="G97" t="n">
-        <v>488.5099535507683</v>
+        <v>470.8719066134257</v>
       </c>
       <c r="H97" t="n">
-        <v>1207.952119063593</v>
+        <v>1320</v>
       </c>
       <c r="I97" t="n">
-        <v>488.5099535507683</v>
+        <v>470.8719066134257</v>
       </c>
       <c r="J97" t="n">
-        <v>1207.952119063593</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="98">
@@ -4585,16 +4585,16 @@
         </is>
       </c>
       <c r="G98" t="n">
-        <v>506.9808142475516</v>
+        <v>442.1199039181038</v>
       </c>
       <c r="H98" t="n">
-        <v>1181.80796508218</v>
+        <v>1200.217232923666</v>
       </c>
       <c r="I98" t="n">
-        <v>506.9808142475516</v>
+        <v>442.1199039181038</v>
       </c>
       <c r="J98" t="n">
-        <v>1181.80796508218</v>
+        <v>1200.217232923666</v>
       </c>
     </row>
     <row r="99">
@@ -4628,13 +4628,13 @@
         <v>540</v>
       </c>
       <c r="H99" t="n">
-        <v>1187.36974110631</v>
+        <v>1320</v>
       </c>
       <c r="I99" t="n">
         <v>540</v>
       </c>
       <c r="J99" t="n">
-        <v>1187.36974110631</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="100">
@@ -4665,16 +4665,16 @@
         </is>
       </c>
       <c r="G100" t="n">
-        <v>515.5823409859667</v>
+        <v>534.6412218880721</v>
       </c>
       <c r="H100" t="n">
-        <v>1236.269823732114</v>
+        <v>1212.009373545457</v>
       </c>
       <c r="I100" t="n">
-        <v>515.5823409859667</v>
+        <v>534.6412218880721</v>
       </c>
       <c r="J100" t="n">
-        <v>1236.269823732114</v>
+        <v>1212.009373545457</v>
       </c>
     </row>
     <row r="101">
@@ -4705,16 +4705,16 @@
         </is>
       </c>
       <c r="G101" t="n">
-        <v>501.8733502154853</v>
+        <v>521.7939643134179</v>
       </c>
       <c r="H101" t="n">
-        <v>1166.983240083073</v>
+        <v>1320</v>
       </c>
       <c r="I101" t="n">
-        <v>501.8733502154853</v>
+        <v>521.7939643134179</v>
       </c>
       <c r="J101" t="n">
-        <v>1166.983240083073</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="102">
@@ -4745,16 +4745,16 @@
         </is>
       </c>
       <c r="G102" t="n">
-        <v>540</v>
+        <v>514.4025903033981</v>
       </c>
       <c r="H102" t="n">
-        <v>1320</v>
+        <v>1124.108893060921</v>
       </c>
       <c r="I102" t="n">
-        <v>540</v>
+        <v>514.4025903033981</v>
       </c>
       <c r="J102" t="n">
-        <v>1320</v>
+        <v>1124.108893060921</v>
       </c>
     </row>
     <row r="103">
@@ -4785,16 +4785,16 @@
         </is>
       </c>
       <c r="G103" t="n">
-        <v>431.345332279926</v>
+        <v>461.9812927639016</v>
       </c>
       <c r="H103" t="n">
-        <v>1191.072948020083</v>
+        <v>1172.624045934155</v>
       </c>
       <c r="I103" t="n">
-        <v>431.345332279926</v>
+        <v>461.9812927639016</v>
       </c>
       <c r="J103" t="n">
-        <v>1191.072948020083</v>
+        <v>1172.624045934155</v>
       </c>
     </row>
     <row r="104">
@@ -4825,16 +4825,16 @@
         </is>
       </c>
       <c r="G104" t="n">
-        <v>507.1797743938082</v>
+        <v>515.8913608250767</v>
       </c>
       <c r="H104" t="n">
-        <v>1320</v>
+        <v>1284.583526912732</v>
       </c>
       <c r="I104" t="n">
-        <v>507.1797743938082</v>
+        <v>515.8913608250767</v>
       </c>
       <c r="J104" t="n">
-        <v>1320</v>
+        <v>1284.583526912732</v>
       </c>
     </row>
     <row r="105">
@@ -4865,16 +4865,16 @@
         </is>
       </c>
       <c r="G105" t="n">
-        <v>503.2908368097868</v>
+        <v>460.8224364018998</v>
       </c>
       <c r="H105" t="n">
-        <v>1320</v>
+        <v>1290.67512070338</v>
       </c>
       <c r="I105" t="n">
-        <v>503.2908368097868</v>
+        <v>460.8224364018998</v>
       </c>
       <c r="J105" t="n">
-        <v>1320</v>
+        <v>1290.67512070338</v>
       </c>
     </row>
     <row r="106">
@@ -4905,16 +4905,16 @@
         </is>
       </c>
       <c r="G106" t="n">
-        <v>492.7975468812764</v>
+        <v>468.4306718928107</v>
       </c>
       <c r="H106" t="n">
-        <v>1127.563397227397</v>
+        <v>1243.417389489702</v>
       </c>
       <c r="I106" t="n">
-        <v>492.7975468812764</v>
+        <v>468.4306718928107</v>
       </c>
       <c r="J106" t="n">
-        <v>1127.563397227397</v>
+        <v>1243.417389489702</v>
       </c>
     </row>
     <row r="107">
@@ -4945,16 +4945,16 @@
         </is>
       </c>
       <c r="G107" t="n">
-        <v>490.9291110666542</v>
+        <v>482.7275997899243</v>
       </c>
       <c r="H107" t="n">
-        <v>1023.348143811229</v>
+        <v>1309.782939259475</v>
       </c>
       <c r="I107" t="n">
-        <v>490.9291110666542</v>
+        <v>482.7275997899243</v>
       </c>
       <c r="J107" t="n">
-        <v>1023.348143811229</v>
+        <v>1309.782939259475</v>
       </c>
     </row>
     <row r="108">
@@ -4985,16 +4985,16 @@
         </is>
       </c>
       <c r="G108" t="n">
-        <v>477.1109014062662</v>
+        <v>483.7659636249438</v>
       </c>
       <c r="H108" t="n">
-        <v>1107.161280044805</v>
+        <v>1306.482690407641</v>
       </c>
       <c r="I108" t="n">
-        <v>477.1109014062662</v>
+        <v>483.7659636249438</v>
       </c>
       <c r="J108" t="n">
-        <v>1107.161280044805</v>
+        <v>1306.482690407641</v>
       </c>
     </row>
     <row r="109">
@@ -5025,16 +5025,16 @@
         </is>
       </c>
       <c r="G109" t="n">
-        <v>486.2784549696033</v>
+        <v>526.7577862183488</v>
       </c>
       <c r="H109" t="n">
-        <v>1207.084294160133</v>
+        <v>1084.144826620822</v>
       </c>
       <c r="I109" t="n">
-        <v>486.2784549696033</v>
+        <v>526.7577862183488</v>
       </c>
       <c r="J109" t="n">
-        <v>1207.084294160133</v>
+        <v>1084.144826620822</v>
       </c>
     </row>
     <row r="110">
@@ -5065,13 +5065,13 @@
         </is>
       </c>
       <c r="G110" t="n">
-        <v>487.0944389733001</v>
+        <v>420.4154303181838</v>
       </c>
       <c r="H110" t="n">
         <v>1320</v>
       </c>
       <c r="I110" t="n">
-        <v>487.0944389733001</v>
+        <v>420.4154303181838</v>
       </c>
       <c r="J110" t="n">
         <v>1320</v>
@@ -5105,16 +5105,16 @@
         </is>
       </c>
       <c r="G111" t="n">
-        <v>472.5542081912803</v>
+        <v>495.0127005632298</v>
       </c>
       <c r="H111" t="n">
-        <v>1273.518638255934</v>
+        <v>1313.848848994793</v>
       </c>
       <c r="I111" t="n">
-        <v>472.5542081912803</v>
+        <v>495.0127005632298</v>
       </c>
       <c r="J111" t="n">
-        <v>1273.518638255934</v>
+        <v>1313.848848994793</v>
       </c>
     </row>
     <row r="112">
@@ -5145,16 +5145,16 @@
         </is>
       </c>
       <c r="G112" t="n">
-        <v>497.6905213055467</v>
+        <v>482.144735561141</v>
       </c>
       <c r="H112" t="n">
-        <v>1020</v>
+        <v>1204.477780890648</v>
       </c>
       <c r="I112" t="n">
-        <v>497.6905213055467</v>
+        <v>482.144735561141</v>
       </c>
       <c r="J112" t="n">
-        <v>1020</v>
+        <v>1204.477780890648</v>
       </c>
     </row>
     <row r="113">
@@ -5185,16 +5185,16 @@
         </is>
       </c>
       <c r="G113" t="n">
-        <v>540</v>
+        <v>487.0350294179971</v>
       </c>
       <c r="H113" t="n">
-        <v>1320</v>
+        <v>1273.126396677593</v>
       </c>
       <c r="I113" t="n">
-        <v>540</v>
+        <v>487.0350294179971</v>
       </c>
       <c r="J113" t="n">
-        <v>1320</v>
+        <v>1273.126396677593</v>
       </c>
     </row>
     <row r="114">
@@ -5221,20 +5221,20 @@
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G114" t="n">
-        <v>523.1647634235019</v>
+        <v>522.3527513936788</v>
       </c>
       <c r="H114" t="n">
-        <v>1422.897613135276</v>
+        <v>1261.556879130403</v>
       </c>
       <c r="I114" t="n">
-        <v>577.4887414565898</v>
+        <v>612.3863018352124</v>
       </c>
       <c r="J114" t="n">
-        <v>1422.897613135276</v>
+        <v>1261.556879130403</v>
       </c>
     </row>
     <row r="115">
@@ -5261,20 +5261,20 @@
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G115" t="n">
-        <v>567.2571247657582</v>
+        <v>539.6741590665906</v>
       </c>
       <c r="H115" t="n">
-        <v>1329.92820662964</v>
+        <v>1196.918345550703</v>
       </c>
       <c r="I115" t="n">
-        <v>677.8239854363669</v>
+        <v>607.8222936751387</v>
       </c>
       <c r="J115" t="n">
-        <v>1329.92820662964</v>
+        <v>1196.918345550703</v>
       </c>
     </row>
     <row r="116">
@@ -5301,20 +5301,20 @@
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G116" t="n">
-        <v>503.3125695587083</v>
+        <v>420</v>
       </c>
       <c r="H116" t="n">
-        <v>1044.192413349959</v>
+        <v>1116.969971925144</v>
       </c>
       <c r="I116" t="n">
-        <v>561.3335937814069</v>
+        <v>487.3256514907878</v>
       </c>
       <c r="J116" t="n">
-        <v>1044.192413349959</v>
+        <v>1116.969971925144</v>
       </c>
     </row>
     <row r="117">
@@ -5341,20 +5341,20 @@
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G117" t="n">
-        <v>473.373561028697</v>
+        <v>420</v>
       </c>
       <c r="H117" t="n">
-        <v>1205.592605007651</v>
+        <v>1198.994586099664</v>
       </c>
       <c r="I117" t="n">
-        <v>566.9802907709251</v>
+        <v>506.9215568577947</v>
       </c>
       <c r="J117" t="n">
-        <v>1205.592605007651</v>
+        <v>1198.994586099664</v>
       </c>
     </row>
     <row r="118">
@@ -5381,20 +5381,20 @@
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G118" t="n">
-        <v>420</v>
+        <v>502.8582139208396</v>
       </c>
       <c r="H118" t="n">
-        <v>1020</v>
+        <v>1096.952643026481</v>
       </c>
       <c r="I118" t="n">
-        <v>480.5407492695625</v>
+        <v>558.5835156325604</v>
       </c>
       <c r="J118" t="n">
-        <v>1020</v>
+        <v>1096.952643026481</v>
       </c>
     </row>
     <row r="119">
@@ -5421,20 +5421,20 @@
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G119" t="n">
-        <v>420</v>
+        <v>533.2303990533665</v>
       </c>
       <c r="H119" t="n">
-        <v>1371.703189544591</v>
+        <v>1130.526811703685</v>
       </c>
       <c r="I119" t="n">
-        <v>458.9940229612305</v>
+        <v>595.3046642525267</v>
       </c>
       <c r="J119" t="n">
-        <v>1371.703189544591</v>
+        <v>1130.526811703685</v>
       </c>
     </row>
     <row r="120">
@@ -5461,20 +5461,20 @@
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G120" t="n">
-        <v>421.4133206450233</v>
+        <v>539.8010360502632</v>
       </c>
       <c r="H120" t="n">
-        <v>1185.025511322994</v>
+        <v>1244.524087660834</v>
       </c>
       <c r="I120" t="n">
-        <v>458.4326865885344</v>
+        <v>604.8293224413165</v>
       </c>
       <c r="J120" t="n">
-        <v>1185.025511322994</v>
+        <v>1244.524087660834</v>
       </c>
     </row>
     <row r="121">
@@ -5501,20 +5501,20 @@
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G121" t="n">
-        <v>463.6178296418903</v>
+        <v>504.5867489100617</v>
       </c>
       <c r="H121" t="n">
-        <v>1158.29083141603</v>
+        <v>1329.457176414986</v>
       </c>
       <c r="I121" t="n">
-        <v>517.5750056937503</v>
+        <v>541.9377316612083</v>
       </c>
       <c r="J121" t="n">
-        <v>1158.29083141603</v>
+        <v>1329.457176414986</v>
       </c>
     </row>
     <row r="122">
@@ -5541,20 +5541,20 @@
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G122" t="n">
-        <v>519.3236960590234</v>
+        <v>455.6850761273734</v>
       </c>
       <c r="H122" t="n">
-        <v>1020</v>
+        <v>1353.727123512428</v>
       </c>
       <c r="I122" t="n">
-        <v>542.455227175305</v>
+        <v>485.9868883640329</v>
       </c>
       <c r="J122" t="n">
-        <v>1020</v>
+        <v>1353.727123512428</v>
       </c>
     </row>
     <row r="123">
@@ -5581,20 +5581,20 @@
       </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G123" t="n">
-        <v>420</v>
+        <v>449.9098886543994</v>
       </c>
       <c r="H123" t="n">
-        <v>1168.114825446693</v>
+        <v>1020</v>
       </c>
       <c r="I123" t="n">
-        <v>527.8236435924736</v>
+        <v>495.4789793551574</v>
       </c>
       <c r="J123" t="n">
-        <v>1168.114825446693</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="124">
@@ -5621,20 +5621,20 @@
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G124" t="n">
-        <v>475.9344095921315</v>
+        <v>441.4180154314537</v>
       </c>
       <c r="H124" t="n">
-        <v>1292.943641144439</v>
+        <v>1020</v>
       </c>
       <c r="I124" t="n">
-        <v>504.1406296545287</v>
+        <v>486.9096866089784</v>
       </c>
       <c r="J124" t="n">
-        <v>1292.943641144439</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="125">
@@ -5661,20 +5661,20 @@
       </c>
       <c r="F125" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G125" t="n">
-        <v>501.0113563579205</v>
+        <v>471.8357223601419</v>
       </c>
       <c r="H125" t="n">
-        <v>1361.339800239773</v>
+        <v>1020</v>
       </c>
       <c r="I125" t="n">
-        <v>548.4967803065897</v>
+        <v>515.5066098114462</v>
       </c>
       <c r="J125" t="n">
-        <v>1361.339800239773</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="126">
@@ -5701,20 +5701,20 @@
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G126" t="n">
-        <v>452.7494219895172</v>
+        <v>497.4128396478596</v>
       </c>
       <c r="H126" t="n">
-        <v>1228.205012865985</v>
+        <v>1283.300675581999</v>
       </c>
       <c r="I126" t="n">
-        <v>556.87093802574</v>
+        <v>592.2821414949863</v>
       </c>
       <c r="J126" t="n">
-        <v>1228.205012865985</v>
+        <v>1283.300675581999</v>
       </c>
     </row>
     <row r="127">
@@ -5741,20 +5741,20 @@
       </c>
       <c r="F127" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G127" t="n">
-        <v>500.3502761097382</v>
+        <v>524.2015725627313</v>
       </c>
       <c r="H127" t="n">
-        <v>1088.175192682754</v>
+        <v>1272.283305544111</v>
       </c>
       <c r="I127" t="n">
-        <v>541.8067373771657</v>
+        <v>607.6315152076038</v>
       </c>
       <c r="J127" t="n">
-        <v>1088.175192682754</v>
+        <v>1272.283305544111</v>
       </c>
     </row>
     <row r="128">
@@ -5781,20 +5781,20 @@
       </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G128" t="n">
-        <v>433.2248705772892</v>
+        <v>600</v>
       </c>
       <c r="H128" t="n">
-        <v>1357.472342104878</v>
+        <v>1020</v>
       </c>
       <c r="I128" t="n">
-        <v>454.3395608582073</v>
+        <v>658.1278098636736</v>
       </c>
       <c r="J128" t="n">
-        <v>1357.472342104878</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="129">
@@ -5821,20 +5821,20 @@
       </c>
       <c r="F129" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G129" t="n">
-        <v>420</v>
+        <v>506.8249230971963</v>
       </c>
       <c r="H129" t="n">
-        <v>1106.718916643896</v>
+        <v>1020</v>
       </c>
       <c r="I129" t="n">
-        <v>441.1381089720581</v>
+        <v>560.827575034229</v>
       </c>
       <c r="J129" t="n">
-        <v>1106.718916643896</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="130">
@@ -5861,20 +5861,20 @@
       </c>
       <c r="F130" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G130" t="n">
-        <v>564.9598491021552</v>
+        <v>500.2567443972179</v>
       </c>
       <c r="H130" t="n">
-        <v>1185.9067934179</v>
+        <v>1249.635857875869</v>
       </c>
       <c r="I130" t="n">
-        <v>616.498809016666</v>
+        <v>575.5726056315209</v>
       </c>
       <c r="J130" t="n">
-        <v>1185.9067934179</v>
+        <v>1249.635857875869</v>
       </c>
     </row>
     <row r="131">
@@ -5901,20 +5901,20 @@
       </c>
       <c r="F131" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G131" t="n">
         <v>420</v>
       </c>
       <c r="H131" t="n">
-        <v>1234.25133897974</v>
+        <v>1283.987500649293</v>
       </c>
       <c r="I131" t="n">
-        <v>478.6460778569243</v>
+        <v>420</v>
       </c>
       <c r="J131" t="n">
-        <v>1234.25133897974</v>
+        <v>1283.987500649293</v>
       </c>
     </row>
     <row r="132">
@@ -5941,20 +5941,20 @@
       </c>
       <c r="F132" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G132" t="n">
-        <v>484.8656698197467</v>
+        <v>425.6001122001073</v>
       </c>
       <c r="H132" t="n">
-        <v>1440</v>
+        <v>1046.329153363762</v>
       </c>
       <c r="I132" t="n">
-        <v>591.8944223918481</v>
+        <v>500.6572168247736</v>
       </c>
       <c r="J132" t="n">
-        <v>1440</v>
+        <v>1046.329153363762</v>
       </c>
     </row>
     <row r="133">
@@ -5981,20 +5981,20 @@
       </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G133" t="n">
-        <v>529.4497494539961</v>
+        <v>495.9529337502319</v>
       </c>
       <c r="H133" t="n">
-        <v>1020</v>
+        <v>1243.571581112389</v>
       </c>
       <c r="I133" t="n">
-        <v>562.3319708985611</v>
+        <v>515.2016925739811</v>
       </c>
       <c r="J133" t="n">
-        <v>1020</v>
+        <v>1243.571581112389</v>
       </c>
     </row>
     <row r="134">
@@ -6021,20 +6021,20 @@
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G134" t="n">
-        <v>494.4037496315186</v>
+        <v>420</v>
       </c>
       <c r="H134" t="n">
-        <v>1232.485709621986</v>
+        <v>1112.772575705978</v>
       </c>
       <c r="I134" t="n">
-        <v>542.0973269901516</v>
+        <v>505.3366959687702</v>
       </c>
       <c r="J134" t="n">
-        <v>1232.485709621986</v>
+        <v>1112.772575705978</v>
       </c>
     </row>
     <row r="135">
@@ -6061,17 +6061,17 @@
       </c>
       <c r="F135" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G135" t="n">
-        <v>600</v>
+        <v>520.9256452121579</v>
       </c>
       <c r="H135" t="n">
         <v>1020</v>
       </c>
       <c r="I135" t="n">
-        <v>680.9282629757315</v>
+        <v>589.2681992557491</v>
       </c>
       <c r="J135" t="n">
         <v>1020</v>
@@ -6101,20 +6101,20 @@
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G136" t="n">
-        <v>508.1909484341273</v>
+        <v>454.894981144185</v>
       </c>
       <c r="H136" t="n">
-        <v>1182.117924882775</v>
+        <v>1100.072434519885</v>
       </c>
       <c r="I136" t="n">
-        <v>600.0825545944111</v>
+        <v>454.894981144185</v>
       </c>
       <c r="J136" t="n">
-        <v>1182.117924882775</v>
+        <v>1100.072434519885</v>
       </c>
     </row>
     <row r="137">
@@ -6141,20 +6141,20 @@
       </c>
       <c r="F137" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G137" t="n">
-        <v>447.9805805162744</v>
+        <v>420</v>
       </c>
       <c r="H137" t="n">
-        <v>1225.747141798899</v>
+        <v>1026.662635686716</v>
       </c>
       <c r="I137" t="n">
-        <v>557.9935541694105</v>
+        <v>465.3609883484278</v>
       </c>
       <c r="J137" t="n">
-        <v>1225.747141798899</v>
+        <v>1026.662635686716</v>
       </c>
     </row>
     <row r="138">
@@ -6181,20 +6181,20 @@
       </c>
       <c r="F138" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G138" t="n">
-        <v>428.1070801019502</v>
+        <v>531.9521028415239</v>
       </c>
       <c r="H138" t="n">
-        <v>1148.825674358548</v>
+        <v>1020</v>
       </c>
       <c r="I138" t="n">
-        <v>522.5810078542484</v>
+        <v>562.3773880919019</v>
       </c>
       <c r="J138" t="n">
-        <v>1148.825674358548</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="139">
@@ -6221,20 +6221,20 @@
       </c>
       <c r="F139" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G139" t="n">
-        <v>458.3694422257848</v>
+        <v>450.6989342104529</v>
       </c>
       <c r="H139" t="n">
-        <v>1202.871584028376</v>
+        <v>1121.777585844562</v>
       </c>
       <c r="I139" t="n">
-        <v>578.3694422257848</v>
+        <v>546.7796816789945</v>
       </c>
       <c r="J139" t="n">
-        <v>1202.871584028376</v>
+        <v>1121.777585844562</v>
       </c>
     </row>
     <row r="140">
@@ -6261,20 +6261,20 @@
       </c>
       <c r="F140" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G140" t="n">
-        <v>420</v>
+        <v>430.0209505601812</v>
       </c>
       <c r="H140" t="n">
-        <v>1192.953875904998</v>
+        <v>1440</v>
       </c>
       <c r="I140" t="n">
-        <v>475.8662244922655</v>
+        <v>506.3723096994649</v>
       </c>
       <c r="J140" t="n">
-        <v>1192.953875904998</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="141">
@@ -6301,20 +6301,20 @@
       </c>
       <c r="F141" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G141" t="n">
-        <v>422.7999359151198</v>
+        <v>490.5299291548017</v>
       </c>
       <c r="H141" t="n">
-        <v>1166.677484088443</v>
+        <v>1185.209971808844</v>
       </c>
       <c r="I141" t="n">
-        <v>502.839199131308</v>
+        <v>562.6822231832537</v>
       </c>
       <c r="J141" t="n">
-        <v>1166.677484088443</v>
+        <v>1185.209971808844</v>
       </c>
     </row>
     <row r="142">
@@ -6341,20 +6341,20 @@
       </c>
       <c r="F142" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G142" t="n">
-        <v>524.1549717092756</v>
+        <v>524.5323136751113</v>
       </c>
       <c r="H142" t="n">
-        <v>1187.863798660333</v>
+        <v>1223.183347519985</v>
       </c>
       <c r="I142" t="n">
-        <v>583.2033932209786</v>
+        <v>597.865158728986</v>
       </c>
       <c r="J142" t="n">
-        <v>1187.863798660333</v>
+        <v>1223.183347519985</v>
       </c>
     </row>
     <row r="143">
@@ -6381,20 +6381,20 @@
       </c>
       <c r="F143" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G143" t="n">
-        <v>557.9242487240143</v>
+        <v>500.7609773865977</v>
       </c>
       <c r="H143" t="n">
-        <v>1166.295721628515</v>
+        <v>1243.155542113614</v>
       </c>
       <c r="I143" t="n">
-        <v>601.1624619553933</v>
+        <v>540.8934715313655</v>
       </c>
       <c r="J143" t="n">
-        <v>1166.295721628515</v>
+        <v>1243.155542113614</v>
       </c>
     </row>
     <row r="144">
@@ -6421,20 +6421,20 @@
       </c>
       <c r="F144" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G144" t="n">
-        <v>575.2427109133193</v>
+        <v>467.5968684425783</v>
       </c>
       <c r="H144" t="n">
-        <v>1059.607611529778</v>
+        <v>1337.167131715169</v>
       </c>
       <c r="I144" t="n">
-        <v>588.5350747265342</v>
+        <v>565.0888525244894</v>
       </c>
       <c r="J144" t="n">
-        <v>1059.607611529778</v>
+        <v>1337.167131715169</v>
       </c>
     </row>
     <row r="145">
@@ -6461,20 +6461,20 @@
       </c>
       <c r="F145" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G145" t="n">
-        <v>484.3388156956037</v>
+        <v>497.4212008993877</v>
       </c>
       <c r="H145" t="n">
-        <v>1140.105414972975</v>
+        <v>1263.148372095628</v>
       </c>
       <c r="I145" t="n">
-        <v>529.9534774370079</v>
+        <v>526.1147761234554</v>
       </c>
       <c r="J145" t="n">
-        <v>1140.105414972975</v>
+        <v>1263.148372095628</v>
       </c>
     </row>
     <row r="146">
@@ -6501,20 +6501,20 @@
       </c>
       <c r="F146" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G146" t="n">
-        <v>517.5408444872414</v>
+        <v>507.0432467258146</v>
       </c>
       <c r="H146" t="n">
-        <v>1034.04143253911</v>
+        <v>1048.848021397108</v>
       </c>
       <c r="I146" t="n">
-        <v>576.0833760894573</v>
+        <v>623.6688605299653</v>
       </c>
       <c r="J146" t="n">
-        <v>1034.04143253911</v>
+        <v>1048.848021397108</v>
       </c>
     </row>
     <row r="147">
@@ -6541,20 +6541,20 @@
       </c>
       <c r="F147" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G147" t="n">
-        <v>439.8613294626766</v>
+        <v>526.5184649609849</v>
       </c>
       <c r="H147" t="n">
-        <v>1206.24134741173</v>
+        <v>1020</v>
       </c>
       <c r="I147" t="n">
-        <v>519.9702086497109</v>
+        <v>591.6117016742932</v>
       </c>
       <c r="J147" t="n">
-        <v>1206.24134741173</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="148">
@@ -6581,20 +6581,20 @@
       </c>
       <c r="F148" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G148" t="n">
-        <v>490.0098256600764</v>
+        <v>475.2234759791494</v>
       </c>
       <c r="H148" t="n">
-        <v>1163.930328364201</v>
+        <v>1294.586883727708</v>
       </c>
       <c r="I148" t="n">
-        <v>551.5606672626534</v>
+        <v>493.3167096395144</v>
       </c>
       <c r="J148" t="n">
-        <v>1163.930328364201</v>
+        <v>1294.586883727708</v>
       </c>
     </row>
     <row r="149">
@@ -6621,20 +6621,20 @@
       </c>
       <c r="F149" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G149" t="n">
-        <v>505.4870087667195</v>
+        <v>498.6628181925736</v>
       </c>
       <c r="H149" t="n">
-        <v>1032.46309197824</v>
+        <v>1020</v>
       </c>
       <c r="I149" t="n">
-        <v>522.3934153444504</v>
+        <v>564.3613416909062</v>
       </c>
       <c r="J149" t="n">
-        <v>1032.46309197824</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="150">
@@ -6661,20 +6661,20 @@
       </c>
       <c r="F150" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G150" t="n">
-        <v>600</v>
+        <v>452.5481172000066</v>
       </c>
       <c r="H150" t="n">
-        <v>1205.776308423441</v>
+        <v>1142.949461154988</v>
       </c>
       <c r="I150" t="n">
-        <v>651.8310019619182</v>
+        <v>545.1589258987337</v>
       </c>
       <c r="J150" t="n">
-        <v>1205.776308423441</v>
+        <v>1142.949461154988</v>
       </c>
     </row>
     <row r="151">
@@ -6701,20 +6701,20 @@
       </c>
       <c r="F151" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G151" t="n">
-        <v>486.0541190806748</v>
+        <v>516.781014361224</v>
       </c>
       <c r="H151" t="n">
-        <v>1351.239292539237</v>
+        <v>1029.863069137863</v>
       </c>
       <c r="I151" t="n">
-        <v>539.4918152274512</v>
+        <v>605.8064892119097</v>
       </c>
       <c r="J151" t="n">
-        <v>1351.239292539237</v>
+        <v>1029.863069137863</v>
       </c>
     </row>
     <row r="152">
@@ -6741,20 +6741,20 @@
       </c>
       <c r="F152" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G152" t="n">
-        <v>465.7304715918485</v>
+        <v>493.8883214469311</v>
       </c>
       <c r="H152" t="n">
-        <v>1274.838903459025</v>
+        <v>1023.886673041734</v>
       </c>
       <c r="I152" t="n">
-        <v>530.7679749950695</v>
+        <v>536.6671189930969</v>
       </c>
       <c r="J152" t="n">
-        <v>1274.838903459025</v>
+        <v>1023.886673041734</v>
       </c>
     </row>
     <row r="153">
@@ -6781,20 +6781,20 @@
       </c>
       <c r="F153" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G153" t="n">
-        <v>600</v>
+        <v>441.2548278919749</v>
       </c>
       <c r="H153" t="n">
-        <v>1108.345122190521</v>
+        <v>1440</v>
       </c>
       <c r="I153" t="n">
-        <v>700.3298120336724</v>
+        <v>510.4802384576539</v>
       </c>
       <c r="J153" t="n">
-        <v>1108.345122190521</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="154">
@@ -6821,20 +6821,20 @@
       </c>
       <c r="F154" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G154" t="n">
-        <v>511.0484298012521</v>
+        <v>422.2627109366722</v>
       </c>
       <c r="H154" t="n">
-        <v>1131.429989559836</v>
+        <v>1020</v>
       </c>
       <c r="I154" t="n">
-        <v>544.9246691858459</v>
+        <v>478.4410442323824</v>
       </c>
       <c r="J154" t="n">
-        <v>1131.429989559836</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="155">
@@ -6861,20 +6861,20 @@
       </c>
       <c r="F155" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G155" t="n">
-        <v>550.9638433980426</v>
+        <v>420</v>
       </c>
       <c r="H155" t="n">
-        <v>1182.115571819252</v>
+        <v>1398.333515645766</v>
       </c>
       <c r="I155" t="n">
-        <v>655.8225631174162</v>
+        <v>524.6106211674297</v>
       </c>
       <c r="J155" t="n">
-        <v>1182.115571819252</v>
+        <v>1398.333515645766</v>
       </c>
     </row>
     <row r="156">
@@ -6901,20 +6901,20 @@
       </c>
       <c r="F156" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G156" t="n">
-        <v>426.215971810165</v>
+        <v>421.7768656759081</v>
       </c>
       <c r="H156" t="n">
-        <v>1020</v>
+        <v>1440</v>
       </c>
       <c r="I156" t="n">
-        <v>512.5028127818332</v>
+        <v>469.3687252004971</v>
       </c>
       <c r="J156" t="n">
-        <v>1020</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="157">
@@ -6941,20 +6941,20 @@
       </c>
       <c r="F157" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G157" t="n">
-        <v>420</v>
+        <v>476.521927377346</v>
       </c>
       <c r="H157" t="n">
-        <v>1160.417605505792</v>
+        <v>1085.601724322185</v>
       </c>
       <c r="I157" t="n">
-        <v>486.0368033959065</v>
+        <v>503.0338589317931</v>
       </c>
       <c r="J157" t="n">
-        <v>1160.417605505792</v>
+        <v>1085.601724322185</v>
       </c>
     </row>
     <row r="158">
@@ -6981,20 +6981,20 @@
       </c>
       <c r="F158" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G158" t="n">
-        <v>516.9568649756609</v>
+        <v>501.8959664253762</v>
       </c>
       <c r="H158" t="n">
-        <v>1102.938616949756</v>
+        <v>1020</v>
       </c>
       <c r="I158" t="n">
-        <v>604.1519443339287</v>
+        <v>579.1338827832116</v>
       </c>
       <c r="J158" t="n">
-        <v>1102.938616949756</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="159">
@@ -7021,20 +7021,20 @@
       </c>
       <c r="F159" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G159" t="n">
-        <v>465.342728502158</v>
+        <v>519.8305680965655</v>
       </c>
       <c r="H159" t="n">
-        <v>1020</v>
+        <v>1423.964833864938</v>
       </c>
       <c r="I159" t="n">
-        <v>523.89242224625</v>
+        <v>538.1410268442023</v>
       </c>
       <c r="J159" t="n">
-        <v>1020</v>
+        <v>1423.964833864938</v>
       </c>
     </row>
     <row r="160">
@@ -7061,20 +7061,20 @@
       </c>
       <c r="F160" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G160" t="n">
-        <v>520.0085985142947</v>
+        <v>485.8606405727646</v>
       </c>
       <c r="H160" t="n">
-        <v>1166.480686715284</v>
+        <v>1440</v>
       </c>
       <c r="I160" t="n">
-        <v>586.9616675152278</v>
+        <v>485.8606405727646</v>
       </c>
       <c r="J160" t="n">
-        <v>1166.480686715284</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="161">
@@ -7101,20 +7101,20 @@
       </c>
       <c r="F161" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G161" t="n">
-        <v>420</v>
+        <v>535.7558000289563</v>
       </c>
       <c r="H161" t="n">
-        <v>1177.840993064951</v>
+        <v>1338.586121844047</v>
       </c>
       <c r="I161" t="n">
-        <v>463.5311082283753</v>
+        <v>586.3570635588447</v>
       </c>
       <c r="J161" t="n">
-        <v>1177.840993064951</v>
+        <v>1338.586121844047</v>
       </c>
     </row>
     <row r="162">
@@ -7141,20 +7141,20 @@
       </c>
       <c r="F162" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G162" t="n">
-        <v>561.8551207687503</v>
+        <v>521.7477190938542</v>
       </c>
       <c r="H162" t="n">
-        <v>1138.645789666388</v>
+        <v>1029.771139645307</v>
       </c>
       <c r="I162" t="n">
-        <v>628.722614577377</v>
+        <v>563.8614906903398</v>
       </c>
       <c r="J162" t="n">
-        <v>1138.645789666388</v>
+        <v>1029.771139645307</v>
       </c>
     </row>
     <row r="163">
@@ -7181,20 +7181,20 @@
       </c>
       <c r="F163" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G163" t="n">
-        <v>422.2346698260536</v>
+        <v>595.2484086256148</v>
       </c>
       <c r="H163" t="n">
-        <v>1020</v>
+        <v>1440</v>
       </c>
       <c r="I163" t="n">
-        <v>510.0581326000214</v>
+        <v>668.8703678314236</v>
       </c>
       <c r="J163" t="n">
-        <v>1020</v>
+        <v>1440</v>
       </c>
     </row>
     <row r="164">
@@ -7221,20 +7221,20 @@
       </c>
       <c r="F164" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G164" t="n">
-        <v>600</v>
+        <v>470.6174155459405</v>
       </c>
       <c r="H164" t="n">
-        <v>1047.571854820889</v>
+        <v>1397.013242759839</v>
       </c>
       <c r="I164" t="n">
-        <v>652.1316632103566</v>
+        <v>527.8836415157377</v>
       </c>
       <c r="J164" t="n">
-        <v>1047.571854820889</v>
+        <v>1397.013242759839</v>
       </c>
     </row>
     <row r="165">
@@ -7261,20 +7261,20 @@
       </c>
       <c r="F165" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G165" t="n">
-        <v>505.5608382916039</v>
+        <v>441.4332249355592</v>
       </c>
       <c r="H165" t="n">
-        <v>1068.072103121416</v>
+        <v>1020</v>
       </c>
       <c r="I165" t="n">
-        <v>552.8380995256111</v>
+        <v>473.2646560837141</v>
       </c>
       <c r="J165" t="n">
-        <v>1068.072103121416</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="166">
@@ -7301,20 +7301,20 @@
       </c>
       <c r="F166" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G166" t="n">
-        <v>551.1162435822962</v>
+        <v>482.4495084849239</v>
       </c>
       <c r="H166" t="n">
-        <v>1182.973254608258</v>
+        <v>1254.135872779253</v>
       </c>
       <c r="I166" t="n">
-        <v>621.9197952963221</v>
+        <v>511.6897239778413</v>
       </c>
       <c r="J166" t="n">
-        <v>1182.973254608258</v>
+        <v>1254.135872779253</v>
       </c>
     </row>
     <row r="167">
@@ -7341,17 +7341,17 @@
       </c>
       <c r="F167" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G167" t="n">
-        <v>528.9823854707773</v>
+        <v>420</v>
       </c>
       <c r="H167" t="n">
         <v>1020</v>
       </c>
       <c r="I167" t="n">
-        <v>638.6340454221466</v>
+        <v>504.4854614187777</v>
       </c>
       <c r="J167" t="n">
         <v>1020</v>
@@ -7381,20 +7381,20 @@
       </c>
       <c r="F168" t="inlineStr">
         <is>
-          <t>entertainment</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="G168" t="n">
-        <v>516.0618460390162</v>
+        <v>511.0391421924672</v>
       </c>
       <c r="H168" t="n">
-        <v>1432.288828396103</v>
+        <v>1344.655174575446</v>
       </c>
       <c r="I168" t="n">
-        <v>516.0618460390162</v>
+        <v>607.4272028864192</v>
       </c>
       <c r="J168" t="n">
-        <v>1432.288828396103</v>
+        <v>1344.655174575446</v>
       </c>
     </row>
   </sheetData>

</xml_diff>